<commit_message>
updated test; little refactoring
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E8DF21-877C-427A-A4EB-050F3EB1FA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C1858A-6497-4824-BF96-CA9798F3DDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="471">
   <si>
     <t>costi acquisti [fissi]</t>
   </si>
@@ -1466,6 +1466,12 @@
   </si>
   <si>
     <t>// cosa fa questo foglio? Se già definito (con name?) modifica scadenza di credito e debito; se non definito, crea un credito/debito vs patrimonio (o vs cash?)</t>
+  </si>
+  <si>
+    <t>$modulesloader</t>
+  </si>
+  <si>
+    <t>https://github.com/77it/financial-modeling/blob/master/src/modules/_modules_loader.js</t>
   </si>
 </sst>
 </file>
@@ -11331,7 +11337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2374C14-97BD-4C0C-A0B9-06A2D874015A}">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -13791,12 +13797,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4483405-5FFC-4EDD-902E-75E3FB56B872}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
     <col min="3" max="3" width="38.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13827,9 +13834,21 @@
         <v>440</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>438</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>469</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>470</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{A198DCAD-25FD-4DA1-99C6-730376022561}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{B2E0B986-CB25-4C33-904D-D50088209C6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update to test asset
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88279114-AC4E-45E0-BA8E-390973E667C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94606CEA-8B81-45CC-9D2B-776B5B7082D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -1468,10 +1468,10 @@
     <t>$modulesloader</t>
   </si>
   <si>
-    <t>https://github.com/77it/financial-modeling/blob/v0.1.22/src/modules/_modules_loader.js</t>
-  </si>
-  <si>
-    <t>https://github.com/77it/financial-modeling/blob/v0.1.22/src/engine/engine.js</t>
+    <t>https://github.com/77it/financial-modeling/blob/v0.1.23/src/engine/engine.js</t>
+  </si>
+  <si>
+    <t>https://github.com/77it/financial-modeling/blob/v0.1.23/src/modules/_modules_loader.js</t>
   </si>
 </sst>
 </file>
@@ -13800,7 +13800,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13833,7 +13833,7 @@
         <v>439</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -13844,7 +13844,7 @@
         <v>468</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moded names used by main.js from Settings to settings_names
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94606CEA-8B81-45CC-9D2B-776B5B7082D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAA4CD7-EBF0-4DA6-8C5C-70660DB28711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -1378,9 +1378,6 @@
     <t>$</t>
   </si>
   <si>
-    <t>$engine</t>
-  </si>
-  <si>
     <t>// -1 means "indefinite" payment schedule</t>
   </si>
   <si>
@@ -1465,13 +1462,16 @@
     <t>// cosa fa questo foglio? Se già definito (con name?) modifica scadenza di credito e debito; se non definito, crea un credito/debito vs patrimonio (o vs cash?)</t>
   </si>
   <si>
-    <t>$modulesloader</t>
-  </si>
-  <si>
     <t>https://github.com/77it/financial-modeling/blob/v0.1.23/src/engine/engine.js</t>
   </si>
   <si>
     <t>https://github.com/77it/financial-modeling/blob/v0.1.23/src/modules/_modules_loader.js</t>
+  </si>
+  <si>
+    <t>$$engine</t>
+  </si>
+  <si>
+    <t>$$modulesloader</t>
   </si>
 </sst>
 </file>
@@ -9239,7 +9239,7 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -9252,7 +9252,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B5" s="52">
         <v>44926</v>
@@ -9264,7 +9264,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7"/>
       <c r="C7" s="51" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="49"/>
@@ -9277,37 +9277,37 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="52"/>
       <c r="C9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="52"/>
       <c r="C10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="52"/>
       <c r="C11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="52"/>
       <c r="C12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="52"/>
       <c r="C13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -9394,10 +9394,10 @@
         <v>117999.24</v>
       </c>
       <c r="C19" t="s">
+        <v>457</v>
+      </c>
+      <c r="E19" s="42" t="s">
         <v>458</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -9408,10 +9408,10 @@
         <v>107617.42</v>
       </c>
       <c r="C20" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -9425,7 +9425,7 @@
         <v>-1</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -11317,7 +11317,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B187" s="50">
         <f>SUBTOTAL(109,CO__crediti2022[31/12/2022])</f>
@@ -11360,7 +11360,7 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -11373,7 +11373,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B5" s="52">
         <v>44926</v>
@@ -11384,7 +11384,7 @@
         <v>433</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
@@ -11393,27 +11393,27 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -11444,7 +11444,7 @@
         <v>-1</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
@@ -11455,7 +11455,7 @@
         <v>695155.84</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>43</v>
@@ -11483,7 +11483,7 @@
         <v>212666.6</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>45</v>
@@ -11497,7 +11497,7 @@
         <v>188072.09</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E19" s="42" t="s">
         <v>46</v>
@@ -11525,7 +11525,7 @@
         <v>145080.97</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>47</v>
@@ -11539,7 +11539,7 @@
         <v>122466.16</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>48</v>
@@ -11581,7 +11581,7 @@
         <v>61600</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>46</v>
@@ -11595,7 +11595,7 @@
         <v>60401.98</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E26" s="42" t="s">
         <v>46</v>
@@ -11609,7 +11609,7 @@
         <v>56309.13</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>46</v>
@@ -11623,7 +11623,7 @@
         <v>55000</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E28" s="42" t="s">
         <v>46</v>
@@ -11651,7 +11651,7 @@
         <v>51146.03</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E30" s="42" t="s">
         <v>46</v>
@@ -11665,7 +11665,7 @@
         <v>49278.57</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E31" s="42" t="s">
         <v>46</v>
@@ -11679,7 +11679,7 @@
         <v>48819.42</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>46</v>
@@ -11693,7 +11693,7 @@
         <v>47580</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>46</v>
@@ -11721,7 +11721,7 @@
         <v>45274.92</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>46</v>
@@ -11735,7 +11735,7 @@
         <v>42355.06</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E36" s="42" t="s">
         <v>46</v>
@@ -11749,7 +11749,7 @@
         <v>42284.11</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>49</v>
@@ -11763,7 +11763,7 @@
         <v>41834.81</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>46</v>
@@ -11791,7 +11791,7 @@
         <v>40543.78</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>50</v>
@@ -11833,7 +11833,7 @@
         <v>34116.22</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E43" s="42" t="s">
         <v>51</v>
@@ -11861,7 +11861,7 @@
         <v>32318.5</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E45" s="42" t="s">
         <v>53</v>
@@ -11875,7 +11875,7 @@
         <v>32108.45</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E46" s="42" t="s">
         <v>51</v>
@@ -11889,7 +11889,7 @@
         <v>30834.65</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E47" s="42" t="s">
         <v>46</v>
@@ -11917,7 +11917,7 @@
         <v>29682.45</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E49" s="42" t="s">
         <v>46</v>
@@ -11931,7 +11931,7 @@
         <v>25000</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E50" s="42" t="s">
         <v>46</v>
@@ -11945,7 +11945,7 @@
         <v>23714.76</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E51" s="42" t="s">
         <v>46</v>
@@ -11959,7 +11959,7 @@
         <v>23213.16</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E52" s="42" t="s">
         <v>46</v>
@@ -11995,7 +11995,7 @@
         <v>18249.57</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E55" s="42" t="s">
         <v>54</v>
@@ -12023,7 +12023,7 @@
         <v>17528.45</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E57" s="42" t="s">
         <v>54</v>
@@ -12051,7 +12051,7 @@
         <v>16367.84</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E59" s="42" t="s">
         <v>55</v>
@@ -12076,7 +12076,7 @@
         <v>15200.9</v>
       </c>
       <c r="C61" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E61" s="42" t="s">
         <v>54</v>
@@ -12118,7 +12118,7 @@
         <v>14875.7</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E64" s="42" t="s">
         <v>56</v>
@@ -12132,7 +12132,7 @@
         <v>14829.63</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E65" s="42" t="s">
         <v>56</v>
@@ -12146,7 +12146,7 @@
         <v>14740.49</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E66" s="42" t="s">
         <v>56</v>
@@ -12160,7 +12160,7 @@
         <v>14420.08</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E67" s="42" t="s">
         <v>56</v>
@@ -12174,7 +12174,7 @@
         <v>14233.58</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E68" s="42" t="s">
         <v>56</v>
@@ -12188,7 +12188,7 @@
         <v>14232.93</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E69" s="42" t="s">
         <v>56</v>
@@ -12202,7 +12202,7 @@
         <v>13750</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E70" s="42" t="s">
         <v>56</v>
@@ -12216,7 +12216,7 @@
         <v>13267.63</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E71" s="42" t="s">
         <v>56</v>
@@ -12241,7 +12241,7 @@
         <v>13123.71</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E73" s="42" t="s">
         <v>56</v>
@@ -12266,7 +12266,7 @@
         <v>11722.92</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E75" s="42" t="s">
         <v>56</v>
@@ -12280,7 +12280,7 @@
         <v>11714.56</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E76" s="42" t="s">
         <v>56</v>
@@ -12294,7 +12294,7 @@
         <v>11680.8</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>56</v>
@@ -12344,7 +12344,7 @@
         <v>10787.57</v>
       </c>
       <c r="C81" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E81" s="42" t="s">
         <v>56</v>
@@ -12369,7 +12369,7 @@
         <v>10463.709999999999</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E83" s="42" t="s">
         <v>56</v>
@@ -12397,7 +12397,7 @@
         <v>9961.4500000000007</v>
       </c>
       <c r="C85" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E85" s="42" t="s">
         <v>57</v>
@@ -12450,7 +12450,7 @@
         <v>9358.25</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E89" s="42" t="s">
         <v>57</v>
@@ -12464,7 +12464,7 @@
         <v>8637.9699999999993</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E90" s="42" t="s">
         <v>57</v>
@@ -12514,7 +12514,7 @@
         <v>7735.25</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E94" s="42" t="s">
         <v>57</v>
@@ -12528,7 +12528,7 @@
         <v>7016.45</v>
       </c>
       <c r="C95" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E95" s="42" t="s">
         <v>57</v>
@@ -12623,7 +12623,7 @@
         <v>5407.75</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E102" s="42" t="s">
         <v>58</v>
@@ -12651,7 +12651,7 @@
         <v>5254.37</v>
       </c>
       <c r="C104" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E104" s="42" t="s">
         <v>58</v>
@@ -12665,7 +12665,7 @@
         <v>5211.95</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E105" s="42" t="s">
         <v>58</v>
@@ -12704,7 +12704,7 @@
         <v>4772.8999999999996</v>
       </c>
       <c r="C108" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E108" s="42" t="s">
         <v>59</v>
@@ -12743,7 +12743,7 @@
         <v>4266.5</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E111" s="42" t="s">
         <v>59</v>
@@ -12779,7 +12779,7 @@
         <v>3828</v>
       </c>
       <c r="C114" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E114" s="42" t="s">
         <v>59</v>
@@ -12804,7 +12804,7 @@
         <v>3614.27</v>
       </c>
       <c r="C116" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>59</v>
@@ -12829,7 +12829,7 @@
         <v>3503.5</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E118" s="42" t="s">
         <v>59</v>
@@ -12843,7 +12843,7 @@
         <v>3409.48</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E119" s="42" t="s">
         <v>59</v>
@@ -12904,7 +12904,7 @@
         <v>3269.64</v>
       </c>
       <c r="C124" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E124" s="42" t="s">
         <v>59</v>
@@ -12918,7 +12918,7 @@
         <v>3040.8</v>
       </c>
       <c r="C125" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E125" s="42" t="s">
         <v>59</v>
@@ -12943,7 +12943,7 @@
         <v>2669.85</v>
       </c>
       <c r="C127" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E127" s="42" t="s">
         <v>60</v>
@@ -12957,7 +12957,7 @@
         <v>2562</v>
       </c>
       <c r="C128" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E128" s="42" t="s">
         <v>60</v>
@@ -13774,7 +13774,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B202" s="50">
         <f>SUBTOTAL(109,CO__debiti2022[31/12/2022])</f>
@@ -13800,7 +13800,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13830,10 +13830,10 @@
         <v>438</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>439</v>
+        <v>469</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -13841,10 +13841,10 @@
         <v>438</v>
       </c>
       <c r="B5" s="47" t="s">
+        <v>470</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>468</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
main: new function to read settings.
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAA4CD7-EBF0-4DA6-8C5C-70660DB28711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714DC273-7556-4A9D-B78D-9813960D8E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="473">
   <si>
     <t>costi acquisti [fissi]</t>
   </si>
@@ -1472,6 +1472,12 @@
   </si>
   <si>
     <t>$$modulesloader</t>
+  </si>
+  <si>
+    <t>$$scenarios</t>
+  </si>
+  <si>
+    <t>['a', 'b']</t>
   </si>
 </sst>
 </file>
@@ -13797,10 +13803,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4483405-5FFC-4EDD-902E-75E3FB56B872}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13830,10 +13836,10 @@
         <v>438</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>469</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>467</v>
+        <v>471</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -13841,16 +13847,27 @@
         <v>438</v>
       </c>
       <c r="B5" s="47" t="s">
+        <v>469</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>438</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>470</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C6" s="48" t="s">
         <v>468</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{A198DCAD-25FD-4DA1-99C6-730376022561}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{B2E0B986-CB25-4C33-904D-D50088209C6F}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{A198DCAD-25FD-4DA1-99C6-730376022561}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{B2E0B986-CB25-4C33-904D-D50088209C6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
settings names: added sanitization. SimulationContextStart, added isDefinedLock.  ismovements, WIP, is the new standard for modules
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1750D254-BE17-46DB-9D50-1B0173B92686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCED1D11-0B35-43A5-ACCF-DA99C1879029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>{intercompany:'aaa', financed:'xxx'} // financed viene scaricato per cassa</t>
   </si>
   <si>
-    <t>$$ mod GenericMovement.Settings</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -1550,6 +1547,9 @@
   </si>
   <si>
     <t>[1,1,3,1,1,1,1,1,1,1,1,5]</t>
+  </si>
+  <si>
+    <t>$$ mod GenericMovements.Settings</t>
   </si>
 </sst>
 </file>
@@ -1993,60 +1993,6 @@
   </cellStyles>
   <dxfs count="40">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2171,6 +2117,60 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3260,7 +3260,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3903D1C0-B8E3-409C-BE95-1255AB23BC7B}" name="Category"/>
     <tableColumn id="2" xr3:uid="{E6C6DD38-D57E-451B-9516-73067D23D77D}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{B2E2BC57-9B61-418F-8C5D-32FDC6C45991}" name="Vs" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B2E2BC57-9B61-418F-8C5D-32FDC6C45991}" name="Vs" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3272,25 +3272,25 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{563511D9-10F8-40C6-B79A-E58B1DE91EE6}" name="Name"/>
     <tableColumn id="2" xr3:uid="{C453AB18-E863-4C2D-8065-F4F105A56E9B}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{C46BCA7A-B736-4054-B024-4832625AFC31}" name="Dilazione" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{F1D3970F-BE94-4966-8D7D-2C33B94E03EE}" name="Ripartizione" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{C46BCA7A-B736-4054-B024-4832625AFC31}" name="Dilazione" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{F1D3970F-BE94-4966-8D7D-2C33B94E03EE}" name="Ripartizione" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A16:E189" totalsRowCount="1" headerRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A16:E189" totalsRowCount="1" headerRowBorderDxfId="13">
   <autoFilter ref="A16:E188" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:B187">
     <sortCondition descending="1" ref="B16:B187"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="31/12/2022" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="31/12/2022" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3308,7 +3308,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}" name="CO__debiti2022" displayName="CO__debiti2022" ref="A16:E204" totalsRowCount="1" dataDxfId="9" headerRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}" name="CO__debiti2022" displayName="CO__debiti2022" ref="A16:E204" totalsRowCount="1" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A16:E203" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}">
     <filterColumn colId="2">
       <filters>
@@ -3321,11 +3321,11 @@
     <sortCondition descending="1" ref="B16:B203"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{92365E0F-7791-44CC-98B1-4C09D8503E9A}" name="Nominativo" totalsRowLabel="Total" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{9617103F-D5E4-4165-A17B-302D5B521D46}" name="31/12/2022" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{8D63E753-E03F-478F-B948-6004CB8D832E}" name="simulation input" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{3FE66DC5-19CD-4B1E-BEF2-0B0CB0D36242}" name="vs // name of related SimObjects" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B3686A29-0F1B-4541-A21D-945F44DC510D}" name="descrizione" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{92365E0F-7791-44CC-98B1-4C09D8503E9A}" name="Nominativo" totalsRowLabel="Total" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9617103F-D5E4-4165-A17B-302D5B521D46}" name="31/12/2022" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{8D63E753-E03F-478F-B948-6004CB8D832E}" name="simulation input" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{3FE66DC5-19CD-4B1E-BEF2-0B0CB0D36242}" name="vs // name of related SimObjects" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B3686A29-0F1B-4541-A21D-945F44DC510D}" name="descrizione" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3634,7 +3634,7 @@
   <dimension ref="A1:CM165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3652,7 +3652,7 @@
   <sheetData>
     <row r="1" spans="1:91" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3"/>
       <c r="E1" s="2"/>
@@ -3742,32 +3742,32 @@
     </row>
     <row r="3" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B4" t="s">
         <v>434</v>
-      </c>
-      <c r="B4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B5" t="s">
         <v>472</v>
-      </c>
-      <c r="B5" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>473</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>474</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:91" x14ac:dyDescent="0.35">
@@ -3776,50 +3776,50 @@
     </row>
     <row r="9" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B9"/>
     </row>
     <row r="10" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C11" s="2">
         <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="12" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>494</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="C12" s="2">
+        <v>90</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>495</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>479</v>
-      </c>
-      <c r="C12" s="2">
-        <v>90</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="13" spans="1:91" x14ac:dyDescent="0.35">
@@ -3832,35 +3832,35 @@
     </row>
     <row r="15" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B15"/>
     </row>
     <row r="16" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B16" t="s">
         <v>476</v>
       </c>
-      <c r="B16" t="s">
-        <v>477</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -3876,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -3884,7 +3884,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -3892,10 +3892,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
+        <v>481</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -3903,7 +3903,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -3911,12 +3911,12 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -3932,13 +3932,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>492</v>
-      </c>
       <c r="C28" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D28" s="4"/>
       <c r="G28" s="2"/>
@@ -3998,37 +3998,37 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B37"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B38" t="s">
         <v>434</v>
-      </c>
-      <c r="B38" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>471</v>
+      </c>
+      <c r="B39" t="s">
         <v>472</v>
-      </c>
-      <c r="B39" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>473</v>
+      </c>
+      <c r="B40" s="52" t="s">
         <v>474</v>
-      </c>
-      <c r="B40" s="52" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B41" s="52">
         <v>44561</v>
@@ -4036,7 +4036,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B42" s="52">
         <v>44926</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B43" s="52">
         <v>45291</v>
@@ -4056,35 +4056,35 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B46"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B47" t="s">
         <v>476</v>
       </c>
-      <c r="B47" t="s">
-        <v>477</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
@@ -4092,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
@@ -4100,7 +4100,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
@@ -4108,7 +4108,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
@@ -4116,10 +4116,10 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
+        <v>481</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
@@ -4127,7 +4127,7 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
@@ -4135,7 +4135,7 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
@@ -4144,13 +4144,13 @@
     </row>
     <row r="58" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="59" spans="1:18" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>6</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61" s="26"/>
       <c r="C61" s="28"/>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B62" s="26"/>
       <c r="C62" s="28"/>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" s="26"/>
       <c r="C63" s="28"/>
@@ -4356,7 +4356,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="26"/>
       <c r="C64" s="28"/>
@@ -4406,7 +4406,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="23"/>
       <c r="C65" s="25"/>
@@ -4456,7 +4456,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="23"/>
       <c r="C66" s="25"/>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" s="23"/>
       <c r="C67" s="25"/>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="25"/>
@@ -5527,7 +5527,7 @@
         <v>1</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C86" s="18">
         <v>29910.9</v>
@@ -5583,7 +5583,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C87" s="18">
         <v>37664.78</v>
@@ -9871,7 +9871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9884,7 +9886,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -9892,29 +9894,29 @@
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>496</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B4" t="s">
         <v>434</v>
-      </c>
-      <c r="B4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B6" s="52">
         <v>44926</v>
@@ -9922,10 +9924,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" t="s">
         <v>470</v>
-      </c>
-      <c r="B7" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -9934,7 +9936,7 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9"/>
       <c r="C9" s="51" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -9943,41 +9945,41 @@
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="52"/>
       <c r="C11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="52"/>
       <c r="C12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="52"/>
       <c r="C13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="52"/>
       <c r="C14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="52"/>
       <c r="C15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -9999,7 +10001,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="30">
         <v>700924.19</v>
@@ -10016,7 +10018,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="30">
         <v>345442.02</v>
@@ -10030,7 +10032,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="30">
         <v>198668.46</v>
@@ -10044,7 +10046,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="30">
         <v>176465.34</v>
@@ -10058,35 +10060,35 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="30">
         <v>117999.24</v>
       </c>
       <c r="C21" t="s">
+        <v>454</v>
+      </c>
+      <c r="E21" s="42" t="s">
         <v>455</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="30">
         <v>107617.42</v>
       </c>
       <c r="C22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="30">
         <v>95233.2</v>
@@ -10095,12 +10097,12 @@
         <v>-1</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="30">
         <v>94237.68</v>
@@ -10114,7 +10116,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="30">
         <v>81829.119999999995</v>
@@ -10128,7 +10130,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="30">
         <v>61570.96</v>
@@ -10142,7 +10144,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="30">
         <v>43840</v>
@@ -10156,7 +10158,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="30">
         <v>39465.78</v>
@@ -10170,7 +10172,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="30">
         <v>30672</v>
@@ -10184,7 +10186,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" s="30">
         <v>25640</v>
@@ -10198,7 +10200,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="30">
         <v>21411</v>
@@ -10212,7 +10214,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="30">
         <v>20909.71</v>
@@ -10226,7 +10228,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="30">
         <v>20659.48</v>
@@ -10240,7 +10242,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="30">
         <v>20000</v>
@@ -10254,7 +10256,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="30">
         <v>18217.2</v>
@@ -10268,7 +10270,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="30">
         <v>16826.16</v>
@@ -10282,7 +10284,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="30">
         <v>16440.96</v>
@@ -10296,7 +10298,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B38" s="30">
         <v>11000</v>
@@ -10310,7 +10312,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" s="30">
         <v>10701.84</v>
@@ -10324,7 +10326,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="30">
         <v>9760</v>
@@ -10335,7 +10337,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="30">
         <v>9496.99</v>
@@ -10349,7 +10351,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" s="30">
         <v>8026.32</v>
@@ -10360,7 +10362,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B43" s="30">
         <v>7799.21</v>
@@ -10374,7 +10376,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" s="30">
         <v>6459.82</v>
@@ -10388,7 +10390,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B45" s="30">
         <v>6173.2</v>
@@ -10402,7 +10404,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B46" s="30">
         <v>6087.59</v>
@@ -10413,7 +10415,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B47" s="30">
         <v>5717.25</v>
@@ -10424,7 +10426,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48" s="30">
         <v>5634.55</v>
@@ -10435,7 +10437,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B49" s="30">
         <v>5537.35</v>
@@ -10449,7 +10451,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="30">
         <v>5413.14</v>
@@ -10463,7 +10465,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B51" s="30">
         <v>4944.91</v>
@@ -10477,7 +10479,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="30">
         <v>4701.28</v>
@@ -10488,7 +10490,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B53" s="30">
         <v>4650.6499999999996</v>
@@ -10502,7 +10504,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B54" s="30">
         <v>4640.88</v>
@@ -10516,7 +10518,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B55" s="30">
         <v>4323</v>
@@ -10530,7 +10532,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B56" s="30">
         <v>4076.19</v>
@@ -10541,7 +10543,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="30">
         <v>3776</v>
@@ -10552,7 +10554,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B58" s="30">
         <v>3658.61</v>
@@ -10563,7 +10565,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B59" s="30">
         <v>3313.48</v>
@@ -10574,7 +10576,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" s="30">
         <v>2937.94</v>
@@ -10585,7 +10587,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="30">
         <v>2906.82</v>
@@ -10596,7 +10598,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="30">
         <v>2867.7</v>
@@ -10607,7 +10609,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="30">
         <v>2554.1</v>
@@ -10618,7 +10620,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B64" s="30">
         <v>2549.1999999999998</v>
@@ -10629,7 +10631,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" s="30">
         <v>2491.7600000000002</v>
@@ -10640,7 +10642,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B66" s="30">
         <v>2460</v>
@@ -10651,7 +10653,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" s="30">
         <v>2440</v>
@@ -10662,7 +10664,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B68" s="30">
         <v>2414.29</v>
@@ -10673,7 +10675,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B69" s="30">
         <v>2379.36</v>
@@ -10684,7 +10686,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" s="30">
         <v>2249.9699999999998</v>
@@ -10695,7 +10697,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B71" s="30">
         <v>2221.5100000000002</v>
@@ -10706,7 +10708,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B72" s="30">
         <v>2038.1</v>
@@ -10717,7 +10719,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B73" s="30">
         <v>2038.1</v>
@@ -10728,7 +10730,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B74" s="30">
         <v>1906.7</v>
@@ -10739,7 +10741,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B75" s="30">
         <v>1859.5</v>
@@ -10750,7 +10752,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B76" s="30">
         <v>1785.96</v>
@@ -10761,7 +10763,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B77" s="30">
         <v>1680.9</v>
@@ -10772,7 +10774,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B78" s="30">
         <v>1652.27</v>
@@ -10783,7 +10785,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B79" s="30">
         <v>1500.6</v>
@@ -10794,7 +10796,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B80" s="30">
         <v>1439.73</v>
@@ -10805,7 +10807,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B81" s="30">
         <v>1429.22</v>
@@ -10816,7 +10818,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B82" s="30">
         <v>1327.96</v>
@@ -10827,7 +10829,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B83" s="30">
         <v>1295.7</v>
@@ -10838,7 +10840,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B84" s="30">
         <v>1243.17</v>
@@ -10849,7 +10851,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B85" s="30">
         <v>1190.6300000000001</v>
@@ -10860,7 +10862,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B86" s="30">
         <v>1145.5999999999999</v>
@@ -10871,7 +10873,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B87" s="30">
         <v>1144.68</v>
@@ -10882,7 +10884,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B88" s="30">
         <v>1033.06</v>
@@ -10893,7 +10895,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B89" s="30">
         <v>985.35</v>
@@ -10904,7 +10906,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B90" s="30">
         <v>983.11</v>
@@ -10915,7 +10917,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B91" s="30">
         <v>908.3</v>
@@ -10926,7 +10928,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B92" s="30">
         <v>903.5</v>
@@ -10937,7 +10939,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B93" s="30">
         <v>897</v>
@@ -10948,7 +10950,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B94" s="30">
         <v>878.4</v>
@@ -10959,7 +10961,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B95" s="30">
         <v>861.47</v>
@@ -10970,7 +10972,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B96" s="30">
         <v>857.97</v>
@@ -10981,7 +10983,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B97" s="30">
         <v>848.79</v>
@@ -10992,7 +10994,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B98" s="30">
         <v>840.46</v>
@@ -11003,7 +11005,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B99" s="30">
         <v>840</v>
@@ -11014,7 +11016,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B100" s="30">
         <v>834.24</v>
@@ -11025,7 +11027,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B101" s="30">
         <v>774.8</v>
@@ -11036,7 +11038,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B102" s="30">
         <v>725.4</v>
@@ -11047,7 +11049,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B103" s="30">
         <v>678.49</v>
@@ -11058,7 +11060,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B104" s="30">
         <v>667.37</v>
@@ -11069,7 +11071,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B105" s="30">
         <v>651.6</v>
@@ -11080,7 +11082,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B106" s="30">
         <v>601.89</v>
@@ -11091,7 +11093,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B107" s="30">
         <v>595</v>
@@ -11102,7 +11104,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B108" s="30">
         <v>578.07000000000005</v>
@@ -11113,7 +11115,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B109" s="30">
         <v>573</v>
@@ -11124,7 +11126,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B110" s="30">
         <v>563.70000000000005</v>
@@ -11135,7 +11137,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B111" s="30">
         <v>536.23</v>
@@ -11146,7 +11148,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B112" s="30">
         <v>521.77</v>
@@ -11157,7 +11159,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B113" s="30">
         <v>491.63</v>
@@ -11168,7 +11170,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B114" s="30">
         <v>491.25</v>
@@ -11179,7 +11181,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B115" s="30">
         <v>481.51</v>
@@ -11190,7 +11192,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B116" s="30">
         <v>474.36</v>
@@ -11201,7 +11203,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B117" s="30">
         <v>433.5</v>
@@ -11212,7 +11214,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B118" s="30">
         <v>425</v>
@@ -11223,7 +11225,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B119" s="30">
         <v>408.82</v>
@@ -11234,7 +11236,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B120" s="30">
         <v>392.35</v>
@@ -11245,7 +11247,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B121" s="30">
         <v>382.24</v>
@@ -11256,7 +11258,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B122" s="30">
         <v>373.02</v>
@@ -11267,7 +11269,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B123" s="30">
         <v>341.43</v>
@@ -11278,7 +11280,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B124" s="30">
         <v>312.56</v>
@@ -11289,7 +11291,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B125" s="30">
         <v>303.05</v>
@@ -11300,7 +11302,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B126" s="30">
         <v>296.98</v>
@@ -11311,7 +11313,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B127" s="30">
         <v>292.8</v>
@@ -11322,7 +11324,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B128" s="30">
         <v>292.8</v>
@@ -11333,7 +11335,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B129" s="30">
         <v>290.92</v>
@@ -11344,7 +11346,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B130" s="30">
         <v>278.89</v>
@@ -11355,7 +11357,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B131" s="30">
         <v>278.20999999999998</v>
@@ -11366,7 +11368,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B132" s="30">
         <v>275.23</v>
@@ -11377,7 +11379,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B133" s="30">
         <v>259.13</v>
@@ -11388,7 +11390,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B134" s="30">
         <v>254.37</v>
@@ -11399,7 +11401,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B135" s="30">
         <v>243.04</v>
@@ -11410,7 +11412,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B136" s="30">
         <v>231.24</v>
@@ -11421,7 +11423,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B137" s="30">
         <v>226.92</v>
@@ -11432,7 +11434,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B138" s="30">
         <v>214.49</v>
@@ -11443,7 +11445,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B139" s="30">
         <v>206.97</v>
@@ -11454,7 +11456,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B140" s="30">
         <v>190.31</v>
@@ -11465,7 +11467,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B141" s="30">
         <v>187.47</v>
@@ -11476,7 +11478,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B142" s="30">
         <v>179.97</v>
@@ -11487,7 +11489,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B143" s="30">
         <v>176.78</v>
@@ -11498,7 +11500,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B144" s="30">
         <v>172.9</v>
@@ -11509,7 +11511,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B145" s="30">
         <v>159.58000000000001</v>
@@ -11520,7 +11522,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B146" s="30">
         <v>136.58000000000001</v>
@@ -11531,7 +11533,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B147" s="30">
         <v>128.31</v>
@@ -11542,7 +11544,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B148" s="30">
         <v>120.38</v>
@@ -11553,7 +11555,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B149" s="30">
         <v>102.48</v>
@@ -11564,7 +11566,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B150" s="30">
         <v>96.94</v>
@@ -11575,7 +11577,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B151" s="30">
         <v>85</v>
@@ -11586,7 +11588,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B152" s="30">
         <v>76.8</v>
@@ -11597,7 +11599,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B153" s="30">
         <v>75.3</v>
@@ -11608,7 +11610,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B154" s="30">
         <v>70.5</v>
@@ -11619,7 +11621,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B155" s="30">
         <v>56</v>
@@ -11630,7 +11632,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B156" s="30">
         <v>55.24</v>
@@ -11641,7 +11643,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B157" s="30">
         <v>54.5</v>
@@ -11652,7 +11654,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B158" s="30">
         <v>51.24</v>
@@ -11663,7 +11665,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B159" s="30">
         <v>50</v>
@@ -11674,7 +11676,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B160" s="30">
         <v>48.17</v>
@@ -11685,7 +11687,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B161" s="30">
         <v>32.11</v>
@@ -11696,7 +11698,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B162" s="30">
         <v>21</v>
@@ -11707,7 +11709,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B163" s="30">
         <v>20</v>
@@ -11718,7 +11720,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B164" s="30">
         <v>18.82</v>
@@ -11729,7 +11731,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B165" s="30">
         <v>17</v>
@@ -11740,7 +11742,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B166" s="30">
         <v>15</v>
@@ -11751,7 +11753,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B167" s="30">
         <v>15</v>
@@ -11762,7 +11764,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B168" s="30">
         <v>14.5</v>
@@ -11773,7 +11775,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B169" s="30">
         <v>14</v>
@@ -11784,7 +11786,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B170" s="30">
         <v>14</v>
@@ -11795,7 +11797,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B171" s="30">
         <v>13.95</v>
@@ -11806,7 +11808,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B172" s="30">
         <v>8.36</v>
@@ -11817,7 +11819,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B173" s="30">
         <v>8</v>
@@ -11828,7 +11830,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B174" s="30">
         <v>0</v>
@@ -11839,7 +11841,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B175" s="30">
         <v>0</v>
@@ -11850,7 +11852,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B176" s="30">
         <v>0</v>
@@ -11861,7 +11863,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B177" s="30">
         <v>0</v>
@@ -11872,7 +11874,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B178" s="30">
         <v>0</v>
@@ -11883,7 +11885,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B179" s="30">
         <v>0</v>
@@ -11894,7 +11896,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B180" s="30">
         <v>-14.15</v>
@@ -11905,7 +11907,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B181" s="30">
         <v>-40.26</v>
@@ -11916,7 +11918,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B182" s="30">
         <v>-128.1</v>
@@ -11927,7 +11929,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B183" s="30">
         <v>-171.29</v>
@@ -11938,7 +11940,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B184" s="30">
         <v>-255.98</v>
@@ -11949,7 +11951,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B185" s="30">
         <v>-512.14</v>
@@ -11960,7 +11962,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B186" s="30">
         <v>-682.43</v>
@@ -11971,7 +11973,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B187" s="30">
         <v>-1975.07</v>
@@ -11987,7 +11989,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B189" s="50">
         <f>SUBTOTAL(109,CO__crediti2022[31/12/2022])</f>
@@ -12008,7 +12010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2374C14-97BD-4C0C-A0B9-06A2D874015A}">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12021,33 +12025,33 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B4" t="s">
         <v>434</v>
-      </c>
-      <c r="B4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B6" s="52">
         <v>44926</v>
@@ -12055,18 +12059,18 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" t="s">
         <v>470</v>
-      </c>
-      <c r="B7" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
@@ -12075,27 +12079,27 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -12117,7 +12121,7 @@
     </row>
     <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B17" s="38">
         <v>851474.64</v>
@@ -12126,18 +12130,18 @@
         <v>-1</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B18" s="38">
         <v>695155.84</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>42</v>
@@ -12145,7 +12149,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B19" s="38">
         <v>244488.74</v>
@@ -12159,13 +12163,13 @@
     </row>
     <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B20" s="38">
         <v>212666.6</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E20" s="42" t="s">
         <v>44</v>
@@ -12173,13 +12177,13 @@
     </row>
     <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B21" s="38">
         <v>188072.09</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>45</v>
@@ -12187,7 +12191,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B22" s="38">
         <v>155343.53</v>
@@ -12201,13 +12205,13 @@
     </row>
     <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B23" s="38">
         <v>145080.97</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E23" s="42" t="s">
         <v>46</v>
@@ -12215,13 +12219,13 @@
     </row>
     <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" s="38">
         <v>122466.16</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>47</v>
@@ -12229,7 +12233,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B25" s="38">
         <v>97260.23</v>
@@ -12243,7 +12247,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B26" s="38">
         <v>81303.12</v>
@@ -12257,13 +12261,13 @@
     </row>
     <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B27" s="38">
         <v>61600</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>45</v>
@@ -12271,13 +12275,13 @@
     </row>
     <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B28" s="38">
         <v>60401.98</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E28" s="42" t="s">
         <v>45</v>
@@ -12285,13 +12289,13 @@
     </row>
     <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B29" s="38">
         <v>56309.13</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E29" s="42" t="s">
         <v>45</v>
@@ -12299,13 +12303,13 @@
     </row>
     <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B30" s="38">
         <v>55000</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E30" s="42" t="s">
         <v>45</v>
@@ -12313,7 +12317,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B31" s="38">
         <v>52175.74</v>
@@ -12327,13 +12331,13 @@
     </row>
     <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B32" s="38">
         <v>51146.03</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>45</v>
@@ -12341,13 +12345,13 @@
     </row>
     <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B33" s="38">
         <v>49278.57</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>45</v>
@@ -12355,13 +12359,13 @@
     </row>
     <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B34" s="38">
         <v>48819.42</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>45</v>
@@ -12369,13 +12373,13 @@
     </row>
     <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B35" s="38">
         <v>47580</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>45</v>
@@ -12383,7 +12387,7 @@
     </row>
     <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B36" s="38">
         <v>46948.49</v>
@@ -12397,13 +12401,13 @@
     </row>
     <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B37" s="38">
         <v>45274.92</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>45</v>
@@ -12411,13 +12415,13 @@
     </row>
     <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B38" s="38">
         <v>42355.06</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>45</v>
@@ -12425,13 +12429,13 @@
     </row>
     <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B39" s="38">
         <v>42284.11</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>48</v>
@@ -12439,13 +12443,13 @@
     </row>
     <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B40" s="38">
         <v>41834.81</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>45</v>
@@ -12453,7 +12457,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B41" s="38">
         <v>40842.949999999997</v>
@@ -12467,13 +12471,13 @@
     </row>
     <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B42" s="38">
         <v>40543.78</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E42" s="42" t="s">
         <v>49</v>
@@ -12481,7 +12485,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B43" s="38">
         <v>38188</v>
@@ -12495,7 +12499,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B44" s="38">
         <v>35428.910000000003</v>
@@ -12509,13 +12513,13 @@
     </row>
     <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B45" s="38">
         <v>34116.22</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E45" s="42" t="s">
         <v>50</v>
@@ -12523,7 +12527,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B46" s="38">
         <v>34030.07</v>
@@ -12537,13 +12541,13 @@
     </row>
     <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B47" s="38">
         <v>32318.5</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E47" s="42" t="s">
         <v>52</v>
@@ -12551,13 +12555,13 @@
     </row>
     <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B48" s="38">
         <v>32108.45</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E48" s="42" t="s">
         <v>50</v>
@@ -12565,13 +12569,13 @@
     </row>
     <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B49" s="38">
         <v>30834.65</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E49" s="42" t="s">
         <v>45</v>
@@ -12579,7 +12583,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B50" s="38">
         <v>29960</v>
@@ -12593,13 +12597,13 @@
     </row>
     <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B51" s="38">
         <v>29682.45</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E51" s="42" t="s">
         <v>45</v>
@@ -12607,13 +12611,13 @@
     </row>
     <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B52" s="38">
         <v>25000</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E52" s="42" t="s">
         <v>45</v>
@@ -12621,13 +12625,13 @@
     </row>
     <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B53" s="38">
         <v>23714.76</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E53" s="42" t="s">
         <v>45</v>
@@ -12635,13 +12639,13 @@
     </row>
     <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B54" s="38">
         <v>23213.16</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E54" s="42" t="s">
         <v>45</v>
@@ -12649,7 +12653,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B55" s="38">
         <v>21177.98</v>
@@ -12660,7 +12664,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B56" s="38">
         <v>18671.919999999998</v>
@@ -12671,13 +12675,13 @@
     </row>
     <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B57" s="38">
         <v>18249.57</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E57" s="42" t="s">
         <v>53</v>
@@ -12685,7 +12689,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B58" s="38">
         <v>17882.759999999998</v>
@@ -12699,13 +12703,13 @@
     </row>
     <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B59" s="38">
         <v>17528.45</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E59" s="42" t="s">
         <v>53</v>
@@ -12713,7 +12717,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B60" s="38">
         <v>17160.95</v>
@@ -12727,13 +12731,13 @@
     </row>
     <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B61" s="38">
         <v>16367.84</v>
       </c>
       <c r="C61" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E61" s="42" t="s">
         <v>54</v>
@@ -12741,7 +12745,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B62" s="38">
         <v>15381.71</v>
@@ -12752,13 +12756,13 @@
     </row>
     <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B63" s="38">
         <v>15200.9</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E63" s="42" t="s">
         <v>53</v>
@@ -12766,7 +12770,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B64" s="38">
         <v>15159.5</v>
@@ -12780,7 +12784,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B65" s="38">
         <v>14981.6</v>
@@ -12794,13 +12798,13 @@
     </row>
     <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B66" s="38">
         <v>14875.7</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E66" s="42" t="s">
         <v>55</v>
@@ -12808,13 +12812,13 @@
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B67" s="38">
         <v>14829.63</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E67" s="42" t="s">
         <v>55</v>
@@ -12822,13 +12826,13 @@
     </row>
     <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B68" s="38">
         <v>14740.49</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E68" s="42" t="s">
         <v>55</v>
@@ -12836,13 +12840,13 @@
     </row>
     <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B69" s="38">
         <v>14420.08</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E69" s="42" t="s">
         <v>55</v>
@@ -12850,13 +12854,13 @@
     </row>
     <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B70" s="38">
         <v>14233.58</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E70" s="42" t="s">
         <v>55</v>
@@ -12864,13 +12868,13 @@
     </row>
     <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B71" s="38">
         <v>14232.93</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E71" s="42" t="s">
         <v>55</v>
@@ -12878,13 +12882,13 @@
     </row>
     <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B72" s="38">
         <v>13750</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E72" s="42" t="s">
         <v>55</v>
@@ -12892,13 +12896,13 @@
     </row>
     <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B73" s="38">
         <v>13267.63</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E73" s="42" t="s">
         <v>55</v>
@@ -12906,7 +12910,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B74" s="38">
         <v>13202</v>
@@ -12917,13 +12921,13 @@
     </row>
     <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B75" s="38">
         <v>13123.71</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E75" s="42" t="s">
         <v>55</v>
@@ -12931,7 +12935,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B76" s="38">
         <v>13084.51</v>
@@ -12942,13 +12946,13 @@
     </row>
     <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B77" s="38">
         <v>11722.92</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>55</v>
@@ -12956,13 +12960,13 @@
     </row>
     <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B78" s="38">
         <v>11714.56</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E78" s="42" t="s">
         <v>55</v>
@@ -12970,13 +12974,13 @@
     </row>
     <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B79" s="38">
         <v>11680.8</v>
       </c>
       <c r="C79" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E79" s="42" t="s">
         <v>55</v>
@@ -12984,7 +12988,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B80" s="38">
         <v>11508.38</v>
@@ -12998,7 +13002,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B81" s="38">
         <v>11316.23</v>
@@ -13009,7 +13013,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B82" s="38">
         <v>11122.71</v>
@@ -13020,13 +13024,13 @@
     </row>
     <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B83" s="38">
         <v>10787.57</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E83" s="42" t="s">
         <v>55</v>
@@ -13034,7 +13038,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B84" s="38">
         <v>10505.28</v>
@@ -13045,13 +13049,13 @@
     </row>
     <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B85" s="38">
         <v>10463.709999999999</v>
       </c>
       <c r="C85" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E85" s="42" t="s">
         <v>55</v>
@@ -13059,7 +13063,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B86" s="38">
         <v>10370</v>
@@ -13073,13 +13077,13 @@
     </row>
     <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B87" s="38">
         <v>9961.4500000000007</v>
       </c>
       <c r="C87" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E87" s="42" t="s">
         <v>56</v>
@@ -13087,7 +13091,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B88" s="38">
         <v>9754.69</v>
@@ -13098,7 +13102,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B89" s="38">
         <v>9563.2900000000009</v>
@@ -13112,7 +13116,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B90" s="38">
         <v>9360.4500000000007</v>
@@ -13126,13 +13130,13 @@
     </row>
     <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B91" s="38">
         <v>9358.25</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E91" s="42" t="s">
         <v>56</v>
@@ -13140,13 +13144,13 @@
     </row>
     <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B92" s="38">
         <v>8637.9699999999993</v>
       </c>
       <c r="C92" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E92" s="42" t="s">
         <v>56</v>
@@ -13154,7 +13158,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B93" s="38">
         <v>8408.93</v>
@@ -13165,7 +13169,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B94" s="38">
         <v>7933.17</v>
@@ -13176,7 +13180,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B95" s="38">
         <v>7924.8</v>
@@ -13190,13 +13194,13 @@
     </row>
     <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B96" s="38">
         <v>7735.25</v>
       </c>
       <c r="C96" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E96" s="42" t="s">
         <v>56</v>
@@ -13204,13 +13208,13 @@
     </row>
     <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B97" s="38">
         <v>7016.45</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E97" s="42" t="s">
         <v>56</v>
@@ -13218,7 +13222,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B98" s="38">
         <v>6832</v>
@@ -13232,7 +13236,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B99" s="38">
         <v>6758.88</v>
@@ -13243,7 +13247,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B100" s="38">
         <v>6093.36</v>
@@ -13257,7 +13261,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B101" s="38">
         <v>5795</v>
@@ -13271,7 +13275,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B102" s="38">
         <v>5764</v>
@@ -13285,7 +13289,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B103" s="38">
         <v>5502.35</v>
@@ -13299,13 +13303,13 @@
     </row>
     <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B104" s="38">
         <v>5407.75</v>
       </c>
       <c r="C104" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E104" s="42" t="s">
         <v>57</v>
@@ -13313,7 +13317,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B105" s="38">
         <v>5342.38</v>
@@ -13327,13 +13331,13 @@
     </row>
     <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B106" s="38">
         <v>5254.37</v>
       </c>
       <c r="C106" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E106" s="42" t="s">
         <v>57</v>
@@ -13341,13 +13345,13 @@
     </row>
     <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B107" s="38">
         <v>5211.95</v>
       </c>
       <c r="C107" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E107" s="42" t="s">
         <v>57</v>
@@ -13355,7 +13359,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B108" s="38">
         <v>5160</v>
@@ -13369,7 +13373,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B109" s="38">
         <v>5032.6000000000004</v>
@@ -13380,13 +13384,13 @@
     </row>
     <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B110" s="38">
         <v>4772.8999999999996</v>
       </c>
       <c r="C110" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E110" s="42" t="s">
         <v>58</v>
@@ -13394,7 +13398,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B111" s="38">
         <v>4538.87</v>
@@ -13405,7 +13409,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B112" s="38">
         <v>4454.6000000000004</v>
@@ -13419,13 +13423,13 @@
     </row>
     <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B113" s="38">
         <v>4266.5</v>
       </c>
       <c r="C113" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E113" s="42" t="s">
         <v>58</v>
@@ -13433,7 +13437,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B114" s="38">
         <v>4254.51</v>
@@ -13444,7 +13448,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B115" s="38">
         <v>4027.16</v>
@@ -13455,13 +13459,13 @@
     </row>
     <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B116" s="38">
         <v>3828</v>
       </c>
       <c r="C116" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>58</v>
@@ -13469,7 +13473,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B117" s="38">
         <v>3733.2</v>
@@ -13480,13 +13484,13 @@
     </row>
     <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B118" s="38">
         <v>3614.27</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E118" s="42" t="s">
         <v>58</v>
@@ -13494,7 +13498,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B119" s="38">
         <v>3524.71</v>
@@ -13505,13 +13509,13 @@
     </row>
     <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B120" s="38">
         <v>3503.5</v>
       </c>
       <c r="C120" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E120" s="42" t="s">
         <v>58</v>
@@ -13519,13 +13523,13 @@
     </row>
     <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B121" s="38">
         <v>3409.48</v>
       </c>
       <c r="C121" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E121" s="42" t="s">
         <v>58</v>
@@ -13533,7 +13537,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B122" s="38">
         <v>3390.99</v>
@@ -13544,7 +13548,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B123" s="38">
         <v>3385.5</v>
@@ -13558,7 +13562,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B124" s="38">
         <v>3355</v>
@@ -13569,7 +13573,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B125" s="38">
         <v>3339.6</v>
@@ -13580,13 +13584,13 @@
     </row>
     <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B126" s="38">
         <v>3269.64</v>
       </c>
       <c r="C126" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E126" s="42" t="s">
         <v>58</v>
@@ -13594,13 +13598,13 @@
     </row>
     <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B127" s="38">
         <v>3040.8</v>
       </c>
       <c r="C127" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E127" s="42" t="s">
         <v>58</v>
@@ -13608,7 +13612,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B128" s="38">
         <v>2869.7</v>
@@ -13619,13 +13623,13 @@
     </row>
     <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B129" s="38">
         <v>2669.85</v>
       </c>
       <c r="C129" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E129" s="42" t="s">
         <v>59</v>
@@ -13633,13 +13637,13 @@
     </row>
     <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B130" s="38">
         <v>2562</v>
       </c>
       <c r="C130" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E130" s="42" t="s">
         <v>59</v>
@@ -13647,7 +13651,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B131" s="38">
         <v>2519.91</v>
@@ -13658,7 +13662,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B132" s="38">
         <v>2501</v>
@@ -13669,7 +13673,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B133" s="38">
         <v>2350.4</v>
@@ -13680,7 +13684,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B134" s="38">
         <v>2217.96</v>
@@ -13691,7 +13695,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B135" s="38">
         <v>2086.1999999999998</v>
@@ -13705,7 +13709,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B136" s="38">
         <v>2080</v>
@@ -13719,7 +13723,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B137" s="38">
         <v>2067.0100000000002</v>
@@ -13730,7 +13734,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B138" s="38">
         <v>2059.36</v>
@@ -13741,7 +13745,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B139" s="38">
         <v>2000</v>
@@ -13752,7 +13756,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B140" s="38">
         <v>1963.25</v>
@@ -13763,7 +13767,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B141" s="38">
         <v>1952</v>
@@ -13774,7 +13778,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B142" s="38">
         <v>1952</v>
@@ -13785,7 +13789,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B143" s="38">
         <v>1769</v>
@@ -13796,7 +13800,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B144" s="38">
         <v>1732</v>
@@ -13807,7 +13811,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B145" s="38">
         <v>1400.56</v>
@@ -13818,7 +13822,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B146" s="38">
         <v>1291.68</v>
@@ -13829,7 +13833,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B147" s="38">
         <v>1105.5999999999999</v>
@@ -13840,7 +13844,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B148" s="38">
         <v>1098</v>
@@ -13851,7 +13855,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B149" s="38">
         <v>1098</v>
@@ -13862,7 +13866,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B150" s="38">
         <v>1083.8499999999999</v>
@@ -13873,7 +13877,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B151" s="38">
         <v>1080</v>
@@ -13884,7 +13888,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B152" s="38">
         <v>1012.6</v>
@@ -13895,7 +13899,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B153" s="38">
         <v>980.98</v>
@@ -13906,7 +13910,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B154" s="38">
         <v>933.3</v>
@@ -13917,7 +13921,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B155" s="38">
         <v>915</v>
@@ -13928,7 +13932,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B156" s="38">
         <v>854</v>
@@ -13939,7 +13943,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B157" s="38">
         <v>829.65</v>
@@ -13950,7 +13954,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B158" s="38">
         <v>805.75</v>
@@ -13961,7 +13965,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B159" s="38">
         <v>788</v>
@@ -13972,7 +13976,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B160" s="38">
         <v>750.4</v>
@@ -13983,7 +13987,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B161" s="38">
         <v>748.8</v>
@@ -13994,7 +13998,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B162" s="38">
         <v>708</v>
@@ -14005,7 +14009,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B163" s="38">
         <v>678</v>
@@ -14016,7 +14020,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B164" s="38">
         <v>613.14</v>
@@ -14027,7 +14031,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B165" s="38">
         <v>585.6</v>
@@ -14038,7 +14042,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B166" s="38">
         <v>582.12</v>
@@ -14049,7 +14053,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B167" s="38">
         <v>492.8</v>
@@ -14060,7 +14064,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B168" s="38">
         <v>491.05</v>
@@ -14071,7 +14075,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B169" s="38">
         <v>488</v>
@@ -14082,7 +14086,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B170" s="38">
         <v>467.5</v>
@@ -14093,7 +14097,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B171" s="38">
         <v>457.5</v>
@@ -14104,7 +14108,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B172" s="38">
         <v>414.8</v>
@@ -14115,7 +14119,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B173" s="38">
         <v>411.4</v>
@@ -14126,7 +14130,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B174" s="38">
         <v>399.9</v>
@@ -14137,7 +14141,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B175" s="38">
         <v>374.7</v>
@@ -14148,7 +14152,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B176" s="38">
         <v>353.12</v>
@@ -14159,7 +14163,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B177" s="38">
         <v>341.6</v>
@@ -14170,7 +14174,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B178" s="38">
         <v>292.8</v>
@@ -14181,7 +14185,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B179" s="38">
         <v>288.64999999999998</v>
@@ -14192,7 +14196,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B180" s="38">
         <v>205.7</v>
@@ -14203,7 +14207,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B181" s="38">
         <v>200.08</v>
@@ -14214,7 +14218,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B182" s="38">
         <v>188.8</v>
@@ -14225,7 +14229,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B183" s="38">
         <v>158.4</v>
@@ -14236,7 +14240,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B184" s="38">
         <v>147.62</v>
@@ -14247,7 +14251,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B185" s="38">
         <v>144</v>
@@ -14258,7 +14262,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B186" s="38">
         <v>128.1</v>
@@ -14269,7 +14273,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B187" s="38">
         <v>123</v>
@@ -14280,7 +14284,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B188" s="38">
         <v>87.65</v>
@@ -14291,7 +14295,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B189" s="38">
         <v>84.91</v>
@@ -14302,7 +14306,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B190" s="38">
         <v>70</v>
@@ -14313,7 +14317,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B191" s="38">
         <v>69.599999999999994</v>
@@ -14324,7 +14328,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B192" s="38">
         <v>48.8</v>
@@ -14335,7 +14339,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B193" s="38">
         <v>47.58</v>
@@ -14346,7 +14350,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B194" s="38">
         <v>46.34</v>
@@ -14357,7 +14361,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B195" s="38">
         <v>30.18</v>
@@ -14368,7 +14372,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B196" s="38">
         <v>11.97</v>
@@ -14379,7 +14383,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B197" s="38">
         <v>0</v>
@@ -14390,7 +14394,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B198" s="38">
         <v>0</v>
@@ -14401,7 +14405,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B199" s="38">
         <v>-42.8</v>
@@ -14412,7 +14416,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B200" s="38">
         <v>-44.01</v>
@@ -14423,7 +14427,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B201" s="38">
         <v>-46.5</v>
@@ -14434,7 +14438,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B202" s="38">
         <v>-555.5</v>
@@ -14445,7 +14449,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B203" s="38">
         <v>-1740</v>
@@ -14456,7 +14460,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B204" s="50">
         <f>SUBTOTAL(109,CO__debiti2022[31/12/2022])</f>
@@ -14494,51 +14498,51 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
+        <v>432</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>433</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="C3" s="45" t="s">
         <v>434</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B4" s="47" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>468</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to modeling. update to search_utils. update to sanitization_utils. corrected bug in agenda + new test.
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F242D-0876-474F-9A3F-14EF12118005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83471A36-2A62-4BA8-B1EE-4A86BB2857BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -1561,13 +1561,13 @@
     <t>Bs_Cash__BankAccount_FinancialAccount</t>
   </si>
   <si>
-    <t>$$ mod IsMovementsH.Settings</t>
-  </si>
-  <si>
     <t>IsMovements(HorizontalDates)</t>
   </si>
   <si>
-    <t>$$ mod GenericMovementsH.Settings</t>
+    <t>$$ mod GenericMovements.Settings</t>
+  </si>
+  <si>
+    <t>$$ mod IsMovements2.Settings</t>
   </si>
 </sst>
 </file>
@@ -2023,30 +2023,6 @@
   </cellStyles>
   <dxfs count="41">
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2085,6 +2061,9 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <fill>
@@ -2142,6 +2121,9 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2165,6 +2147,24 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3301,24 +3301,24 @@
     <tableColumn id="1" xr3:uid="{563511D9-10F8-40C6-B79A-E58B1DE91EE6}" name="Name"/>
     <tableColumn id="2" xr3:uid="{C453AB18-E863-4C2D-8065-F4F105A56E9B}" name="Type"/>
     <tableColumn id="3" xr3:uid="{C46BCA7A-B736-4054-B024-4832625AFC31}" name="Dilazione" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F1D3970F-BE94-4966-8D7D-2C33B94E03EE}" name="split" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F1D3970F-BE94-4966-8D7D-2C33B94E03EE}" name="split" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:E188" totalsRowCount="1" headerRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:E188" totalsRowCount="1" headerRowBorderDxfId="13">
   <autoFilter ref="A15:E187" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:B186">
     <sortCondition descending="1" ref="B15:B186"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3336,7 +3336,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}" name="CO__debiti2022" displayName="CO__debiti2022" ref="A15:E203" totalsRowCount="1" dataDxfId="8" headerRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}" name="CO__debiti2022" displayName="CO__debiti2022" ref="A15:E203" totalsRowCount="1" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A15:E202" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}">
     <filterColumn colId="2">
       <filters>
@@ -3349,11 +3349,11 @@
     <sortCondition descending="1" ref="B15:B202"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{92365E0F-7791-44CC-98B1-4C09D8503E9A}" name="Nominativo" totalsRowLabel="Total" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{9617103F-D5E4-4165-A17B-302D5B521D46}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="0" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{8D63E753-E03F-478F-B948-6004CB8D832E}" name="simulation input" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{3FE66DC5-19CD-4B1E-BEF2-0B0CB0D36242}" name="vs // name of related SimObjects" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B3686A29-0F1B-4541-A21D-945F44DC510D}" name="descrizione" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{92365E0F-7791-44CC-98B1-4C09D8503E9A}" name="Nominativo" totalsRowLabel="Total" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9617103F-D5E4-4165-A17B-302D5B521D46}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{8D63E753-E03F-478F-B948-6004CB8D832E}" name="simulation input" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{3FE66DC5-19CD-4B1E-BEF2-0B0CB0D36242}" name="vs // name of related SimObjects" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B3686A29-0F1B-4541-A21D-945F44DC510D}" name="descrizione" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3672,7 +3672,9 @@
   </sheetPr>
   <dimension ref="A1:CM152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3791,7 +3793,7 @@
     </row>
     <row r="5" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>477</v>
+        <v>502</v>
       </c>
       <c r="B5"/>
     </row>
@@ -3959,7 +3961,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="55" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
@@ -3971,7 +3973,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>500</v>
+        <v>477</v>
       </c>
       <c r="B27"/>
     </row>
@@ -9888,7 +9890,7 @@
   <dimension ref="A1:G188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9910,7 +9912,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B3"/>
     </row>
@@ -12018,7 +12020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2374C14-97BD-4C0C-A0B9-06A2D874015A}">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12036,7 +12040,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -14484,9 +14488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4483405-5FFC-4EDD-902E-75E3FB56B872}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
moving some config to /config/engine.js. edits to excel input test.
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83471A36-2A62-4BA8-B1EE-4A86BB2857BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797861A9-E596-44F2-9CF9-1958286E5AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="506">
   <si>
     <t>costi acquisti [fissi]</t>
   </si>
@@ -1568,6 +1568,15 @@
   </si>
   <si>
     <t>$$ mod IsMovements2.Settings</t>
+  </si>
+  <si>
+    <t>// come opera questo modulo? Se SimObject è già definito (con name) modifica scadenza di credito e debito; se non definito, crea un credito/debito vs "vs type"</t>
+  </si>
+  <si>
+    <t>amount delta value</t>
+  </si>
+  <si>
+    <t>se presente la colonna "simulation input", escludi dalla simulazione righe dove "simulation input" = nullOrWhitespace; se per errore nella riga di totale c'è scritto qualcosa anche sulla riga di "simulation input" allora verrà presa, ma è inevitabile.</t>
   </si>
 </sst>
 </file>
@@ -2021,7 +2030,52 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="45">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2119,9 +2173,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -3232,27 +3283,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E64329F-9E29-4147-93C7-0043B684883A}" name="CO__costi_ricavi" displayName="CO__costi_ricavi" ref="A47:R152" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E64329F-9E29-4147-93C7-0043B684883A}" name="CO__costi_ricavi" displayName="CO__costi_ricavi" ref="A47:R152" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" dataCellStyle="Percent">
   <autoFilter ref="A47:R152" xr:uid="{81DBB65E-D085-4009-B87E-1D8FC1BC5735}"/>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{5424E4F3-82DC-43EC-82CC-5D77DDB2DE4F}" name="Category" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{FC02796A-5245-4E19-98CD-135052708445}" name="Note" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{A3F41BE3-2534-46F8-B22E-22307A5F0632}" name="#2021-12-31" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{3788870B-400A-4276-B51C-05E302B302B8}" name="#2022-12-31" dataDxfId="33"/>
-    <tableColumn id="19" xr3:uid="{A8105DD8-E3E0-4DB6-8920-B834A21B94F4}" name="#2023-12-31" dataDxfId="32" dataCellStyle="Percent"/>
-    <tableColumn id="13" xr3:uid="{7ED33282-BB82-468F-8309-4EF648641D17}" name="giorni di dilazione" dataDxfId="31" dataCellStyle="Percent"/>
-    <tableColumn id="20" xr3:uid="{3878498B-CA3A-438B-9E59-63200D40F101}" name="gen" dataDxfId="30" dataCellStyle="Percent"/>
-    <tableColumn id="21" xr3:uid="{33D5AA8A-D27C-4A01-A9BA-A8141E7B5EA8}" name="feb" dataDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="22" xr3:uid="{EE43375B-8632-4CB0-B2EF-37EC9B0F9BAF}" name="mar" dataDxfId="28" dataCellStyle="Percent"/>
-    <tableColumn id="23" xr3:uid="{7548EF3A-EAE3-4025-ACBC-643E27D805D4}" name="apr" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="24" xr3:uid="{7789B300-28A7-4A07-BDF1-3AFDBB8245A1}" name="mag" dataDxfId="26" dataCellStyle="Percent"/>
-    <tableColumn id="25" xr3:uid="{B12FAB0C-603B-4713-B022-308B4968C990}" name="giu" dataDxfId="25" dataCellStyle="Percent"/>
-    <tableColumn id="26" xr3:uid="{AF786059-8D5C-4117-B4EB-6D53B3ECC153}" name="lug" dataDxfId="24" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{A3F3C0CA-AD61-4E46-AB1E-299BCCCE3599}" name="ago" dataDxfId="23" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{BF1D7492-9E68-4A57-AACE-066B04DD0160}" name="set" dataDxfId="22" dataCellStyle="Percent"/>
-    <tableColumn id="10" xr3:uid="{E9D4ECA1-19D4-4A5C-B423-57987C2A224E}" name="ott" dataDxfId="21" dataCellStyle="Percent"/>
-    <tableColumn id="11" xr3:uid="{0985029D-7C0E-4E80-95D0-E72ECF205469}" name="nov" dataDxfId="20" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{3440EC54-31C0-4B29-997E-E7E578A37AF3}" name="dic" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{5424E4F3-82DC-43EC-82CC-5D77DDB2DE4F}" name="Category" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{FC02796A-5245-4E19-98CD-135052708445}" name="Note" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{A3F41BE3-2534-46F8-B22E-22307A5F0632}" name="#2021-12-31" dataDxfId="38"/>
+    <tableColumn id="14" xr3:uid="{3788870B-400A-4276-B51C-05E302B302B8}" name="#2022-12-31" dataDxfId="37"/>
+    <tableColumn id="19" xr3:uid="{A8105DD8-E3E0-4DB6-8920-B834A21B94F4}" name="#2023-12-31" dataDxfId="36" dataCellStyle="Percent"/>
+    <tableColumn id="13" xr3:uid="{7ED33282-BB82-468F-8309-4EF648641D17}" name="giorni di dilazione" dataDxfId="35" dataCellStyle="Percent"/>
+    <tableColumn id="20" xr3:uid="{3878498B-CA3A-438B-9E59-63200D40F101}" name="gen" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="21" xr3:uid="{33D5AA8A-D27C-4A01-A9BA-A8141E7B5EA8}" name="feb" dataDxfId="33" dataCellStyle="Percent"/>
+    <tableColumn id="22" xr3:uid="{EE43375B-8632-4CB0-B2EF-37EC9B0F9BAF}" name="mar" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="23" xr3:uid="{7548EF3A-EAE3-4025-ACBC-643E27D805D4}" name="apr" dataDxfId="31" dataCellStyle="Percent"/>
+    <tableColumn id="24" xr3:uid="{7789B300-28A7-4A07-BDF1-3AFDBB8245A1}" name="mag" dataDxfId="30" dataCellStyle="Percent"/>
+    <tableColumn id="25" xr3:uid="{B12FAB0C-603B-4713-B022-308B4968C990}" name="giu" dataDxfId="29" dataCellStyle="Percent"/>
+    <tableColumn id="26" xr3:uid="{AF786059-8D5C-4117-B4EB-6D53B3ECC153}" name="lug" dataDxfId="28" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{A3F3C0CA-AD61-4E46-AB1E-299BCCCE3599}" name="ago" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{BF1D7492-9E68-4A57-AACE-066B04DD0160}" name="set" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="10" xr3:uid="{E9D4ECA1-19D4-4A5C-B423-57987C2A224E}" name="ott" dataDxfId="25" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{0985029D-7C0E-4E80-95D0-E72ECF205469}" name="nov" dataDxfId="24" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{3440EC54-31C0-4B29-997E-E7E578A37AF3}" name="dic" dataDxfId="23" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3275,9 +3326,9 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{60D92ED1-E564-4F0E-92D4-ED72B91C2DEB}" name="Category"/>
     <tableColumn id="2" xr3:uid="{C7BDDFAB-3DC8-479E-B176-DB44B3FE3058}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{76F08DB3-7E58-40FD-A9E9-CBBE1DAE8F18}" name="Vs" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{8211519F-6B31-4D41-86E7-B4E338144DEC}" name="Dilazione" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{8DF49F45-F4F9-42F5-80C3-953F525E310A}" name="split" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{76F08DB3-7E58-40FD-A9E9-CBBE1DAE8F18}" name="Vs" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{8211519F-6B31-4D41-86E7-B4E338144DEC}" name="Dilazione" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{8DF49F45-F4F9-42F5-80C3-953F525E310A}" name="split" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3300,33 +3351,35 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{563511D9-10F8-40C6-B79A-E58B1DE91EE6}" name="Name"/>
     <tableColumn id="2" xr3:uid="{C453AB18-E863-4C2D-8065-F4F105A56E9B}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{C46BCA7A-B736-4054-B024-4832625AFC31}" name="Dilazione" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F1D3970F-BE94-4966-8D7D-2C33B94E03EE}" name="split" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{C46BCA7A-B736-4054-B024-4832625AFC31}" name="Dilazione" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{F1D3970F-BE94-4966-8D7D-2C33B94E03EE}" name="split" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:E188" totalsRowCount="1" headerRowBorderDxfId="13">
-  <autoFilter ref="A15:E187" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:B186">
-    <sortCondition descending="1" ref="B15:B186"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A16:G189" totalsRowCount="1" headerRowBorderDxfId="17">
+  <autoFilter ref="A16:G188" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:B187">
+    <sortCondition descending="1" ref="B16:B187"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{0122F6E9-ACDE-4D2E-9536-72D393C72211}" name="type" dataDxfId="3" totalsRowDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{DD0E2DD3-375A-45F2-98AB-836E8D4A9DD6}" name="vs type" dataDxfId="4" totalsRowDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5A97148D-0FD8-41E1-B9E9-5B2818AF7142}" name="Table5" displayName="Table5" ref="A4:B6" totalsRowShown="0">
-  <autoFilter ref="A4:B6" xr:uid="{5A97148D-0FD8-41E1-B9E9-5B2818AF7142}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5A97148D-0FD8-41E1-B9E9-5B2818AF7142}" name="Table5" displayName="Table5" ref="A4:B7" totalsRowShown="0">
+  <autoFilter ref="A4:B7" xr:uid="{5A97148D-0FD8-41E1-B9E9-5B2818AF7142}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{43C4539B-72CD-422C-9B54-B9B23D4937E2}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FBCA0C9B-B4A6-4441-B0BF-BE55DBE98AF6}" name="Value"/>
@@ -3336,7 +3389,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}" name="CO__debiti2022" displayName="CO__debiti2022" ref="A15:E203" totalsRowCount="1" dataDxfId="6" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}" name="CO__debiti2022" displayName="CO__debiti2022" ref="A15:E203" totalsRowCount="1" dataDxfId="11" headerRowBorderDxfId="12">
   <autoFilter ref="A15:E202" xr:uid="{E5601ADE-B24A-49C1-BC43-41BA241A28FA}">
     <filterColumn colId="2">
       <filters>
@@ -3349,11 +3402,11 @@
     <sortCondition descending="1" ref="B15:B202"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{92365E0F-7791-44CC-98B1-4C09D8503E9A}" name="Nominativo" totalsRowLabel="Total" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9617103F-D5E4-4165-A17B-302D5B521D46}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{8D63E753-E03F-478F-B948-6004CB8D832E}" name="simulation input" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{3FE66DC5-19CD-4B1E-BEF2-0B0CB0D36242}" name="vs // name of related SimObjects" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{B3686A29-0F1B-4541-A21D-945F44DC510D}" name="descrizione" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{92365E0F-7791-44CC-98B1-4C09D8503E9A}" name="Nominativo" totalsRowLabel="Total" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{9617103F-D5E4-4165-A17B-302D5B521D46}" name="#2022-12-31" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{8D63E753-E03F-478F-B948-6004CB8D832E}" name="simulation input" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{3FE66DC5-19CD-4B1E-BEF2-0B0CB0D36242}" name="vs // name of related SimObjects" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{B3686A29-0F1B-4541-A21D-945F44DC510D}" name="descrizione" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3672,7 +3725,7 @@
   </sheetPr>
   <dimension ref="A1:CM152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="101" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -9887,2126 +9940,2171 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
-  <dimension ref="A1:G188"/>
+  <dimension ref="A1:I189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="68.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1796875" customWidth="1"/>
-    <col min="5" max="5" width="49.08984375" customWidth="1"/>
+    <col min="2" max="4" width="15.54296875" style="30" customWidth="1"/>
+    <col min="5" max="5" width="68.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" customWidth="1"/>
+    <col min="7" max="7" width="49.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="30"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>428</v>
       </c>
       <c r="B4" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>59</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C6"/>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>498</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7"/>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8"/>
-      <c r="C8" s="50" t="s">
-        <v>452</v>
-      </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="C8"/>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" s="50" t="s">
+        <v>505</v>
+      </c>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B9"/>
-      <c r="C9" t="s">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="51"/>
-      <c r="C10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="51"/>
-      <c r="C11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="51"/>
-      <c r="C12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="51"/>
-      <c r="C13" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="51"/>
-      <c r="C14" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B16" s="57" t="s">
         <v>487</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>498</v>
+      </c>
+      <c r="E16" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="F16" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="G16" s="35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B17" s="30">
         <v>700924.19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E17" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F17" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="G17" s="41" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B18" s="30">
         <v>345442.02</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E18" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="G18" s="41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B19" s="30">
         <v>198668.46</v>
       </c>
-      <c r="C18">
-        <v>90</v>
-      </c>
-      <c r="E18" s="41" t="s">
+      <c r="E19">
+        <v>90</v>
+      </c>
+      <c r="G19" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B20" s="30">
         <v>176465.34</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E20" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="G20" s="41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B21" s="30">
         <v>117999.24</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E21" t="s">
         <v>449</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="G21" s="41" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B22" s="30">
         <v>107617.42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E22" t="s">
         <v>450</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="G22" s="41" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B23" s="30">
         <v>95233.2</v>
       </c>
-      <c r="C22">
+      <c r="E23">
         <v>-1</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="G23" s="41" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B24" s="30">
         <v>94237.68</v>
       </c>
-      <c r="C23">
-        <v>60</v>
-      </c>
-      <c r="E23" s="41" t="s">
+      <c r="E24">
+        <v>60</v>
+      </c>
+      <c r="G24" s="41" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B25" s="30">
         <v>81829.119999999995</v>
       </c>
-      <c r="C24">
-        <v>90</v>
-      </c>
-      <c r="E24" s="41" t="s">
+      <c r="E25">
+        <v>90</v>
+      </c>
+      <c r="G25" s="41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B26" s="30">
         <v>61570.96</v>
       </c>
-      <c r="C25">
+      <c r="E26">
         <v>30</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="G26" s="41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B27" s="30">
         <v>43840</v>
       </c>
-      <c r="C26">
-        <v>60</v>
-      </c>
-      <c r="E26" s="41" t="s">
+      <c r="E27">
+        <v>60</v>
+      </c>
+      <c r="G27" s="41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B28" s="30">
         <v>39465.78</v>
       </c>
-      <c r="C27">
-        <v>60</v>
-      </c>
-      <c r="E27" s="41" t="s">
+      <c r="E28">
+        <v>60</v>
+      </c>
+      <c r="G28" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B29" s="30">
         <v>30672</v>
       </c>
-      <c r="C28">
-        <v>60</v>
-      </c>
-      <c r="E28" s="41" t="s">
+      <c r="E29">
+        <v>60</v>
+      </c>
+      <c r="G29" s="41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B30" s="30">
         <v>25640</v>
       </c>
-      <c r="C29">
-        <v>60</v>
-      </c>
-      <c r="E29" s="41" t="s">
+      <c r="E30">
+        <v>60</v>
+      </c>
+      <c r="G30" s="41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B31" s="30">
         <v>21411</v>
       </c>
-      <c r="C30">
-        <v>60</v>
-      </c>
-      <c r="E30" s="41" t="s">
+      <c r="E31">
+        <v>60</v>
+      </c>
+      <c r="G31" s="41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="30">
+      <c r="B32" s="30">
         <v>20909.71</v>
       </c>
-      <c r="C31">
-        <v>60</v>
-      </c>
-      <c r="E31" s="41" t="s">
+      <c r="E32">
+        <v>60</v>
+      </c>
+      <c r="G32" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="30">
+      <c r="B33" s="30">
         <v>20659.48</v>
       </c>
-      <c r="C32">
-        <v>60</v>
-      </c>
-      <c r="E32" s="41" t="s">
+      <c r="E33">
+        <v>60</v>
+      </c>
+      <c r="G33" s="41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="30">
+      <c r="B34" s="30">
         <v>20000</v>
       </c>
-      <c r="C33">
-        <v>60</v>
-      </c>
-      <c r="E33" s="41" t="s">
+      <c r="E34">
+        <v>60</v>
+      </c>
+      <c r="G34" s="41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B35" s="30">
         <v>18217.2</v>
       </c>
-      <c r="C34">
-        <v>60</v>
-      </c>
-      <c r="E34" s="41" t="s">
+      <c r="E35">
+        <v>60</v>
+      </c>
+      <c r="G35" s="41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B36" s="30">
         <v>16826.16</v>
       </c>
-      <c r="C35">
-        <v>60</v>
-      </c>
-      <c r="E35" s="41" t="s">
+      <c r="E36">
+        <v>60</v>
+      </c>
+      <c r="G36" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B37" s="30">
         <v>16440.96</v>
       </c>
-      <c r="C36">
-        <v>60</v>
-      </c>
-      <c r="E36" s="41" t="s">
+      <c r="E37">
+        <v>60</v>
+      </c>
+      <c r="G37" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B38" s="30">
         <v>11000</v>
       </c>
-      <c r="C37">
-        <v>60</v>
-      </c>
-      <c r="E37" s="41" t="s">
+      <c r="E38">
+        <v>60</v>
+      </c>
+      <c r="G38" s="41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B39" s="30">
         <v>10701.84</v>
       </c>
-      <c r="C38">
-        <v>60</v>
-      </c>
-      <c r="E38" s="41" t="s">
+      <c r="E39">
+        <v>60</v>
+      </c>
+      <c r="G39" s="41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="30">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="30">
         <v>9760</v>
       </c>
-      <c r="C39">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="E40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B41" s="30">
         <v>9496.99</v>
       </c>
-      <c r="C40">
-        <v>60</v>
-      </c>
-      <c r="E40" s="41" t="s">
+      <c r="E41">
+        <v>60</v>
+      </c>
+      <c r="G41" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B42" s="30">
         <v>8026.32</v>
       </c>
-      <c r="C41">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="E42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B43" s="30">
         <v>7799.21</v>
       </c>
-      <c r="C42">
-        <v>60</v>
-      </c>
-      <c r="E42" s="41" t="s">
+      <c r="E43">
+        <v>60</v>
+      </c>
+      <c r="G43" s="41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B44" s="30">
         <v>6459.82</v>
       </c>
-      <c r="C43">
-        <v>60</v>
-      </c>
-      <c r="E43" s="41" t="s">
+      <c r="E44">
+        <v>60</v>
+      </c>
+      <c r="G44" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="30">
+      <c r="B45" s="30">
         <v>6173.2</v>
       </c>
-      <c r="C44">
-        <v>60</v>
-      </c>
-      <c r="E44" s="41" t="s">
+      <c r="E45">
+        <v>60</v>
+      </c>
+      <c r="G45" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="30">
+      <c r="B46" s="30">
         <v>6087.59</v>
       </c>
-      <c r="C45">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="E46">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B47" s="30">
         <v>5717.25</v>
       </c>
-      <c r="C46">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="E47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B48" s="30">
         <v>5634.55</v>
       </c>
-      <c r="C47">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="E48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B49" s="30">
         <v>5537.35</v>
       </c>
-      <c r="C48">
-        <v>60</v>
-      </c>
-      <c r="E48" s="41" t="s">
+      <c r="E49">
+        <v>60</v>
+      </c>
+      <c r="G49" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="30">
+      <c r="B50" s="30">
         <v>5413.14</v>
       </c>
-      <c r="C49">
-        <v>60</v>
-      </c>
-      <c r="E49" s="41" t="s">
+      <c r="E50">
+        <v>60</v>
+      </c>
+      <c r="G50" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B51" s="30">
         <v>4944.91</v>
       </c>
-      <c r="C50">
-        <v>60</v>
-      </c>
-      <c r="E50" s="41" t="s">
+      <c r="E51">
+        <v>60</v>
+      </c>
+      <c r="G51" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="30">
+      <c r="B52" s="30">
         <v>4701.28</v>
       </c>
-      <c r="C51">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="E52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="30">
+      <c r="B53" s="30">
         <v>4650.6499999999996</v>
       </c>
-      <c r="C52">
-        <v>60</v>
-      </c>
-      <c r="E52" s="41" t="s">
+      <c r="E53">
+        <v>60</v>
+      </c>
+      <c r="G53" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="30">
+      <c r="B54" s="30">
         <v>4640.88</v>
       </c>
-      <c r="C53">
-        <v>60</v>
-      </c>
-      <c r="E53" s="41" t="s">
+      <c r="E54">
+        <v>60</v>
+      </c>
+      <c r="G54" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="30">
+      <c r="B55" s="30">
         <v>4323</v>
       </c>
-      <c r="C54">
-        <v>60</v>
-      </c>
-      <c r="E54" s="41" t="s">
+      <c r="E55">
+        <v>60</v>
+      </c>
+      <c r="G55" s="41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="30">
+      <c r="B56" s="30">
         <v>4076.19</v>
       </c>
-      <c r="C55">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="E56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="30">
+      <c r="B57" s="30">
         <v>3776</v>
       </c>
-      <c r="C56">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="E57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="30">
+      <c r="B58" s="30">
         <v>3658.61</v>
       </c>
-      <c r="C57">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="E58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="30">
+      <c r="B59" s="30">
         <v>3313.48</v>
       </c>
-      <c r="C58">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="E59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="30">
+      <c r="B60" s="30">
         <v>2937.94</v>
       </c>
-      <c r="C59">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="E60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="30">
+      <c r="B61" s="30">
         <v>2906.82</v>
       </c>
-      <c r="C60">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+      <c r="E61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>112</v>
       </c>
-      <c r="B61" s="30">
+      <c r="B62" s="30">
         <v>2867.7</v>
       </c>
-      <c r="C61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="E62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="30">
+      <c r="B63" s="30">
         <v>2554.1</v>
       </c>
-      <c r="C62">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+      <c r="E63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="30">
+      <c r="B64" s="30">
         <v>2549.1999999999998</v>
       </c>
-      <c r="C63">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+      <c r="E64">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="30">
+      <c r="B65" s="30">
         <v>2491.7600000000002</v>
       </c>
-      <c r="C64">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="E65">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="30">
+      <c r="B66" s="30">
         <v>2460</v>
       </c>
-      <c r="C65">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="E66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>117</v>
       </c>
-      <c r="B66" s="30">
+      <c r="B67" s="30">
         <v>2440</v>
       </c>
-      <c r="C66">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+      <c r="E67">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>118</v>
       </c>
-      <c r="B67" s="30">
+      <c r="B68" s="30">
         <v>2414.29</v>
       </c>
-      <c r="C67">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+      <c r="E68">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="30">
+      <c r="B69" s="30">
         <v>2379.36</v>
       </c>
-      <c r="C68">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+      <c r="E69">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="30">
+      <c r="B70" s="30">
         <v>2249.9699999999998</v>
       </c>
-      <c r="C69">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+      <c r="E70">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>121</v>
       </c>
-      <c r="B70" s="30">
+      <c r="B71" s="30">
         <v>2221.5100000000002</v>
       </c>
-      <c r="C70">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+      <c r="E71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>122</v>
-      </c>
-      <c r="B71" s="30">
-        <v>2038.1</v>
-      </c>
-      <c r="C71">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>123</v>
       </c>
       <c r="B72" s="30">
         <v>2038.1</v>
       </c>
-      <c r="C72">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E72">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" s="30">
+        <v>2038.1</v>
+      </c>
+      <c r="E73">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>124</v>
       </c>
-      <c r="B73" s="30">
+      <c r="B74" s="30">
         <v>1906.7</v>
       </c>
-      <c r="C73">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+      <c r="E74">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>125</v>
       </c>
-      <c r="B74" s="30">
+      <c r="B75" s="30">
         <v>1859.5</v>
       </c>
-      <c r="C74">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+      <c r="E75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>126</v>
       </c>
-      <c r="B75" s="30">
+      <c r="B76" s="30">
         <v>1785.96</v>
       </c>
-      <c r="C75">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+      <c r="E76">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>127</v>
       </c>
-      <c r="B76" s="30">
+      <c r="B77" s="30">
         <v>1680.9</v>
       </c>
-      <c r="C76">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+      <c r="E77">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>128</v>
       </c>
-      <c r="B77" s="30">
+      <c r="B78" s="30">
         <v>1652.27</v>
       </c>
-      <c r="C77">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+      <c r="E78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>129</v>
       </c>
-      <c r="B78" s="30">
+      <c r="B79" s="30">
         <v>1500.6</v>
       </c>
-      <c r="C78">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+      <c r="E79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>130</v>
       </c>
-      <c r="B79" s="30">
+      <c r="B80" s="30">
         <v>1439.73</v>
       </c>
-      <c r="C79">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+      <c r="E80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>131</v>
       </c>
-      <c r="B80" s="30">
+      <c r="B81" s="30">
         <v>1429.22</v>
       </c>
-      <c r="C80">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+      <c r="E81">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>132</v>
       </c>
-      <c r="B81" s="30">
+      <c r="B82" s="30">
         <v>1327.96</v>
       </c>
-      <c r="C81">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="E82">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>133</v>
       </c>
-      <c r="B82" s="30">
+      <c r="B83" s="30">
         <v>1295.7</v>
       </c>
-      <c r="C82">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="E83">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>134</v>
       </c>
-      <c r="B83" s="30">
+      <c r="B84" s="30">
         <v>1243.17</v>
       </c>
-      <c r="C83">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="E84">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>135</v>
       </c>
-      <c r="B84" s="30">
+      <c r="B85" s="30">
         <v>1190.6300000000001</v>
       </c>
-      <c r="C84">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="E85">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>136</v>
       </c>
-      <c r="B85" s="30">
+      <c r="B86" s="30">
         <v>1145.5999999999999</v>
       </c>
-      <c r="C85">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+      <c r="E86">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>137</v>
       </c>
-      <c r="B86" s="30">
+      <c r="B87" s="30">
         <v>1144.68</v>
       </c>
-      <c r="C86">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+      <c r="E87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>138</v>
       </c>
-      <c r="B87" s="30">
+      <c r="B88" s="30">
         <v>1033.06</v>
       </c>
-      <c r="C87">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+      <c r="E88">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>139</v>
       </c>
-      <c r="B88" s="30">
+      <c r="B89" s="30">
         <v>985.35</v>
       </c>
-      <c r="C88">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+      <c r="E89">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>140</v>
       </c>
-      <c r="B89" s="30">
+      <c r="B90" s="30">
         <v>983.11</v>
       </c>
-      <c r="C89">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+      <c r="E90">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>141</v>
       </c>
-      <c r="B90" s="30">
+      <c r="B91" s="30">
         <v>908.3</v>
       </c>
-      <c r="C90">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="E91">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>142</v>
       </c>
-      <c r="B91" s="30">
+      <c r="B92" s="30">
         <v>903.5</v>
       </c>
-      <c r="C91">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="E92">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>143</v>
       </c>
-      <c r="B92" s="30">
+      <c r="B93" s="30">
         <v>897</v>
       </c>
-      <c r="C92">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="E93">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>144</v>
       </c>
-      <c r="B93" s="30">
+      <c r="B94" s="30">
         <v>878.4</v>
       </c>
-      <c r="C93">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+      <c r="E94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>145</v>
       </c>
-      <c r="B94" s="30">
+      <c r="B95" s="30">
         <v>861.47</v>
       </c>
-      <c r="C94">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="E95">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>146</v>
       </c>
-      <c r="B95" s="30">
+      <c r="B96" s="30">
         <v>857.97</v>
       </c>
-      <c r="C95">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+      <c r="E96">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>147</v>
       </c>
-      <c r="B96" s="30">
+      <c r="B97" s="30">
         <v>848.79</v>
       </c>
-      <c r="C96">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+      <c r="E97">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>148</v>
       </c>
-      <c r="B97" s="30">
+      <c r="B98" s="30">
         <v>840.46</v>
       </c>
-      <c r="C97">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+      <c r="E98">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>149</v>
       </c>
-      <c r="B98" s="30">
+      <c r="B99" s="30">
         <v>840</v>
       </c>
-      <c r="C98">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+      <c r="E99">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>150</v>
       </c>
-      <c r="B99" s="30">
+      <c r="B100" s="30">
         <v>834.24</v>
       </c>
-      <c r="C99">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+      <c r="E100">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>151</v>
       </c>
-      <c r="B100" s="30">
+      <c r="B101" s="30">
         <v>774.8</v>
       </c>
-      <c r="C100">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+      <c r="E101">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>152</v>
       </c>
-      <c r="B101" s="30">
+      <c r="B102" s="30">
         <v>725.4</v>
       </c>
-      <c r="C101">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+      <c r="E102">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>153</v>
       </c>
-      <c r="B102" s="30">
+      <c r="B103" s="30">
         <v>678.49</v>
       </c>
-      <c r="C102">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+      <c r="E103">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>154</v>
       </c>
-      <c r="B103" s="30">
+      <c r="B104" s="30">
         <v>667.37</v>
       </c>
-      <c r="C103">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+      <c r="E104">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>155</v>
       </c>
-      <c r="B104" s="30">
+      <c r="B105" s="30">
         <v>651.6</v>
       </c>
-      <c r="C104">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+      <c r="E105">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>156</v>
       </c>
-      <c r="B105" s="30">
+      <c r="B106" s="30">
         <v>601.89</v>
       </c>
-      <c r="C105">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+      <c r="E106">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>157</v>
       </c>
-      <c r="B106" s="30">
+      <c r="B107" s="30">
         <v>595</v>
       </c>
-      <c r="C106">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+      <c r="E107">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>158</v>
       </c>
-      <c r="B107" s="30">
+      <c r="B108" s="30">
         <v>578.07000000000005</v>
       </c>
-      <c r="C107">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+      <c r="E108">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>159</v>
       </c>
-      <c r="B108" s="30">
+      <c r="B109" s="30">
         <v>573</v>
       </c>
-      <c r="C108">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+      <c r="E109">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>160</v>
       </c>
-      <c r="B109" s="30">
+      <c r="B110" s="30">
         <v>563.70000000000005</v>
       </c>
-      <c r="C109">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+      <c r="E110">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>161</v>
       </c>
-      <c r="B110" s="30">
+      <c r="B111" s="30">
         <v>536.23</v>
       </c>
-      <c r="C110">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+      <c r="E111">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>162</v>
       </c>
-      <c r="B111" s="30">
+      <c r="B112" s="30">
         <v>521.77</v>
       </c>
-      <c r="C111">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+      <c r="E112">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>163</v>
       </c>
-      <c r="B112" s="30">
+      <c r="B113" s="30">
         <v>491.63</v>
       </c>
-      <c r="C112">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+      <c r="E113">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>164</v>
       </c>
-      <c r="B113" s="30">
+      <c r="B114" s="30">
         <v>491.25</v>
       </c>
-      <c r="C113">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+      <c r="E114">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>165</v>
       </c>
-      <c r="B114" s="30">
+      <c r="B115" s="30">
         <v>481.51</v>
       </c>
-      <c r="C114">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+      <c r="E115">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>166</v>
       </c>
-      <c r="B115" s="30">
+      <c r="B116" s="30">
         <v>474.36</v>
       </c>
-      <c r="C115">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+      <c r="E116">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>167</v>
       </c>
-      <c r="B116" s="30">
+      <c r="B117" s="30">
         <v>433.5</v>
       </c>
-      <c r="C116">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+      <c r="E117">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>168</v>
       </c>
-      <c r="B117" s="30">
+      <c r="B118" s="30">
         <v>425</v>
       </c>
-      <c r="C117">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+      <c r="E118">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>169</v>
       </c>
-      <c r="B118" s="30">
+      <c r="B119" s="30">
         <v>408.82</v>
       </c>
-      <c r="C118">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+      <c r="E119">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>170</v>
       </c>
-      <c r="B119" s="30">
+      <c r="B120" s="30">
         <v>392.35</v>
       </c>
-      <c r="C119">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+      <c r="E120">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>171</v>
       </c>
-      <c r="B120" s="30">
+      <c r="B121" s="30">
         <v>382.24</v>
       </c>
-      <c r="C120">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+      <c r="E121">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>172</v>
       </c>
-      <c r="B121" s="30">
+      <c r="B122" s="30">
         <v>373.02</v>
       </c>
-      <c r="C121">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+      <c r="E122">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>173</v>
       </c>
-      <c r="B122" s="30">
+      <c r="B123" s="30">
         <v>341.43</v>
       </c>
-      <c r="C122">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+      <c r="E123">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>174</v>
       </c>
-      <c r="B123" s="30">
+      <c r="B124" s="30">
         <v>312.56</v>
       </c>
-      <c r="C123">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+      <c r="E124">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>175</v>
       </c>
-      <c r="B124" s="30">
+      <c r="B125" s="30">
         <v>303.05</v>
       </c>
-      <c r="C124">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+      <c r="E125">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>176</v>
       </c>
-      <c r="B125" s="30">
+      <c r="B126" s="30">
         <v>296.98</v>
       </c>
-      <c r="C125">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+      <c r="E126">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>177</v>
-      </c>
-      <c r="B126" s="30">
-        <v>292.8</v>
-      </c>
-      <c r="C126">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
-        <v>178</v>
       </c>
       <c r="B127" s="30">
         <v>292.8</v>
       </c>
-      <c r="C127">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E127">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>178</v>
+      </c>
+      <c r="B128" s="30">
+        <v>292.8</v>
+      </c>
+      <c r="E128">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>179</v>
       </c>
-      <c r="B128" s="30">
+      <c r="B129" s="30">
         <v>290.92</v>
       </c>
-      <c r="C128">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+      <c r="E129">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>180</v>
       </c>
-      <c r="B129" s="30">
+      <c r="B130" s="30">
         <v>278.89</v>
       </c>
-      <c r="C129">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="E130">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>181</v>
       </c>
-      <c r="B130" s="30">
+      <c r="B131" s="30">
         <v>278.20999999999998</v>
       </c>
-      <c r="C130">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+      <c r="E131">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>182</v>
       </c>
-      <c r="B131" s="30">
+      <c r="B132" s="30">
         <v>275.23</v>
       </c>
-      <c r="C131">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+      <c r="E132">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>183</v>
       </c>
-      <c r="B132" s="30">
+      <c r="B133" s="30">
         <v>259.13</v>
       </c>
-      <c r="C132">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+      <c r="E133">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>184</v>
       </c>
-      <c r="B133" s="30">
+      <c r="B134" s="30">
         <v>254.37</v>
       </c>
-      <c r="C133">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+      <c r="E134">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>185</v>
       </c>
-      <c r="B134" s="30">
+      <c r="B135" s="30">
         <v>243.04</v>
       </c>
-      <c r="C134">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+      <c r="E135">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>186</v>
       </c>
-      <c r="B135" s="30">
+      <c r="B136" s="30">
         <v>231.24</v>
       </c>
-      <c r="C135">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+      <c r="E136">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>187</v>
       </c>
-      <c r="B136" s="30">
+      <c r="B137" s="30">
         <v>226.92</v>
       </c>
-      <c r="C136">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+      <c r="E137">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>188</v>
       </c>
-      <c r="B137" s="30">
+      <c r="B138" s="30">
         <v>214.49</v>
       </c>
-      <c r="C137">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+      <c r="E138">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>189</v>
       </c>
-      <c r="B138" s="30">
+      <c r="B139" s="30">
         <v>206.97</v>
       </c>
-      <c r="C138">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+      <c r="E139">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>190</v>
       </c>
-      <c r="B139" s="30">
+      <c r="B140" s="30">
         <v>190.31</v>
       </c>
-      <c r="C139">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+      <c r="E140">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>191</v>
       </c>
-      <c r="B140" s="30">
+      <c r="B141" s="30">
         <v>187.47</v>
       </c>
-      <c r="C140">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+      <c r="E141">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>192</v>
       </c>
-      <c r="B141" s="30">
+      <c r="B142" s="30">
         <v>179.97</v>
       </c>
-      <c r="C141">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+      <c r="E142">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>193</v>
       </c>
-      <c r="B142" s="30">
+      <c r="B143" s="30">
         <v>176.78</v>
       </c>
-      <c r="C142">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+      <c r="E143">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>194</v>
       </c>
-      <c r="B143" s="30">
+      <c r="B144" s="30">
         <v>172.9</v>
       </c>
-      <c r="C143">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+      <c r="E144">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>195</v>
       </c>
-      <c r="B144" s="30">
+      <c r="B145" s="30">
         <v>159.58000000000001</v>
       </c>
-      <c r="C144">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+      <c r="E145">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>196</v>
       </c>
-      <c r="B145" s="30">
+      <c r="B146" s="30">
         <v>136.58000000000001</v>
       </c>
-      <c r="C145">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+      <c r="E146">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>197</v>
       </c>
-      <c r="B146" s="30">
+      <c r="B147" s="30">
         <v>128.31</v>
       </c>
-      <c r="C146">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+      <c r="E147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>198</v>
       </c>
-      <c r="B147" s="30">
+      <c r="B148" s="30">
         <v>120.38</v>
       </c>
-      <c r="C147">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+      <c r="E148">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>199</v>
       </c>
-      <c r="B148" s="30">
+      <c r="B149" s="30">
         <v>102.48</v>
       </c>
-      <c r="C148">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+      <c r="E149">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>424</v>
       </c>
-      <c r="B149" s="30">
+      <c r="B150" s="30">
         <v>96.94</v>
       </c>
-      <c r="C149">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+      <c r="E150">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>200</v>
       </c>
-      <c r="B150" s="30">
+      <c r="B151" s="30">
         <v>85</v>
       </c>
-      <c r="C150">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+      <c r="E151">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>201</v>
       </c>
-      <c r="B151" s="30">
+      <c r="B152" s="30">
         <v>76.8</v>
       </c>
-      <c r="C151">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+      <c r="E152">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>202</v>
       </c>
-      <c r="B152" s="30">
+      <c r="B153" s="30">
         <v>75.3</v>
       </c>
-      <c r="C152">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+      <c r="E153">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>203</v>
       </c>
-      <c r="B153" s="30">
+      <c r="B154" s="30">
         <v>70.5</v>
       </c>
-      <c r="C153">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+      <c r="E154">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>204</v>
       </c>
-      <c r="B154" s="30">
+      <c r="B155" s="30">
         <v>56</v>
       </c>
-      <c r="C154">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+      <c r="E155">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>205</v>
       </c>
-      <c r="B155" s="30">
+      <c r="B156" s="30">
         <v>55.24</v>
       </c>
-      <c r="C155">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+      <c r="E156">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>206</v>
       </c>
-      <c r="B156" s="30">
+      <c r="B157" s="30">
         <v>54.5</v>
       </c>
-      <c r="C156">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+      <c r="E157">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>207</v>
       </c>
-      <c r="B157" s="30">
+      <c r="B158" s="30">
         <v>51.24</v>
       </c>
-      <c r="C157">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
+      <c r="E158">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>208</v>
       </c>
-      <c r="B158" s="30">
+      <c r="B159" s="30">
         <v>50</v>
       </c>
-      <c r="C158">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
+      <c r="E159">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>209</v>
       </c>
-      <c r="B159" s="30">
+      <c r="B160" s="30">
         <v>48.17</v>
       </c>
-      <c r="C159">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
+      <c r="E160">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
         <v>210</v>
       </c>
-      <c r="B160" s="30">
+      <c r="B161" s="30">
         <v>32.11</v>
       </c>
-      <c r="C160">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+      <c r="E161">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>211</v>
       </c>
-      <c r="B161" s="30">
+      <c r="B162" s="30">
         <v>21</v>
       </c>
-      <c r="C161">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+      <c r="E162">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
         <v>212</v>
       </c>
-      <c r="B162" s="30">
+      <c r="B163" s="30">
         <v>20</v>
       </c>
-      <c r="C162">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+      <c r="E163">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>213</v>
       </c>
-      <c r="B163" s="30">
+      <c r="B164" s="30">
         <v>18.82</v>
       </c>
-      <c r="C163">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+      <c r="E164">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="30">
+      <c r="B165" s="30">
         <v>17</v>
       </c>
-      <c r="C164">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+      <c r="E165">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
         <v>215</v>
-      </c>
-      <c r="B165" s="30">
-        <v>15</v>
-      </c>
-      <c r="C165">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
-        <v>216</v>
       </c>
       <c r="B166" s="30">
         <v>15</v>
       </c>
-      <c r="C166">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E166">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>216</v>
+      </c>
+      <c r="B167" s="30">
+        <v>15</v>
+      </c>
+      <c r="E167">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
         <v>217</v>
       </c>
-      <c r="B167" s="30">
+      <c r="B168" s="30">
         <v>14.5</v>
       </c>
-      <c r="C167">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+      <c r="E168">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
         <v>218</v>
-      </c>
-      <c r="B168" s="30">
-        <v>14</v>
-      </c>
-      <c r="C168">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
-        <v>219</v>
       </c>
       <c r="B169" s="30">
         <v>14</v>
       </c>
-      <c r="C169">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E169">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>219</v>
+      </c>
+      <c r="B170" s="30">
+        <v>14</v>
+      </c>
+      <c r="E170">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
         <v>220</v>
       </c>
-      <c r="B170" s="30">
+      <c r="B171" s="30">
         <v>13.95</v>
       </c>
-      <c r="C170">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+      <c r="E171">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
         <v>221</v>
       </c>
-      <c r="B171" s="30">
+      <c r="B172" s="30">
         <v>8.36</v>
       </c>
-      <c r="C171">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+      <c r="E172">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
         <v>222</v>
       </c>
-      <c r="B172" s="30">
+      <c r="B173" s="30">
         <v>8</v>
       </c>
-      <c r="C172">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+      <c r="E173">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
         <v>223</v>
-      </c>
-      <c r="B173" s="30">
-        <v>0</v>
-      </c>
-      <c r="C173">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
-        <v>224</v>
       </c>
       <c r="B174" s="30">
         <v>0</v>
       </c>
-      <c r="C174">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E174">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B175" s="30">
         <v>0</v>
       </c>
-      <c r="C175">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E175">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B176" s="30">
         <v>0</v>
       </c>
-      <c r="C176">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E176">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B177" s="30">
         <v>0</v>
       </c>
-      <c r="C177">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E177">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B178" s="30">
         <v>0</v>
       </c>
-      <c r="C178">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E178">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>228</v>
+      </c>
+      <c r="B179" s="30">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
         <v>229</v>
       </c>
-      <c r="B179" s="30">
+      <c r="B180" s="30">
         <v>-14.15</v>
       </c>
-      <c r="C179">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
+      <c r="E180">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
         <v>230</v>
       </c>
-      <c r="B180" s="30">
+      <c r="B181" s="30">
         <v>-40.26</v>
       </c>
-      <c r="C180">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
+      <c r="E181">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
         <v>231</v>
       </c>
-      <c r="B181" s="30">
+      <c r="B182" s="30">
         <v>-128.1</v>
       </c>
-      <c r="C181">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
+      <c r="E182">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
         <v>232</v>
       </c>
-      <c r="B182" s="30">
+      <c r="B183" s="30">
         <v>-171.29</v>
       </c>
-      <c r="C182">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
+      <c r="E183">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
         <v>233</v>
       </c>
-      <c r="B183" s="30">
+      <c r="B184" s="30">
         <v>-255.98</v>
       </c>
-      <c r="C183">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
+      <c r="E184">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
         <v>234</v>
       </c>
-      <c r="B184" s="30">
+      <c r="B185" s="30">
         <v>-512.14</v>
       </c>
-      <c r="C184">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
+      <c r="E185">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
         <v>235</v>
       </c>
-      <c r="B185" s="30">
+      <c r="B186" s="30">
         <v>-682.43</v>
       </c>
-      <c r="C185">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
+      <c r="E186">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
         <v>236</v>
       </c>
-      <c r="B186" s="30">
+      <c r="B187" s="30">
         <v>-1975.07</v>
       </c>
-      <c r="C186">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C187">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
+      <c r="E187">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E188">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
         <v>451</v>
       </c>
-      <c r="B188" s="49">
+      <c r="B189" s="49">
         <f>SUBTOTAL(109,CO__crediti2022['#2022-12-31])</f>
         <v>2471912.100000001</v>
       </c>
+      <c r="C189" s="49"/>
+      <c r="D189" s="49"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>